<commit_message>
Phase-1 Commit and Push
</commit_message>
<xml_diff>
--- a/Excels/KE.xlsx
+++ b/Excels/KE.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="159">
   <si>
     <t>loginAuuid</t>
   </si>
@@ -493,6 +493,30 @@
   </si>
   <si>
     <t>230720001056</t>
+  </si>
+  <si>
+    <t>240720001004</t>
+  </si>
+  <si>
+    <t>240720001005</t>
+  </si>
+  <si>
+    <t>240720001006</t>
+  </si>
+  <si>
+    <t>240720001007</t>
+  </si>
+  <si>
+    <t>240720001008</t>
+  </si>
+  <si>
+    <t>240720001009</t>
+  </si>
+  <si>
+    <t>240720001010</t>
+  </si>
+  <si>
+    <t>240720001011</t>
   </si>
 </sst>
 </file>
@@ -1277,7 +1301,7 @@
         <v>96</v>
       </c>
       <c r="Y2" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.2">
@@ -1324,7 +1348,7 @@
         <v>96</v>
       </c>
       <c r="Y3" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.2">
@@ -1371,7 +1395,7 @@
         <v>96</v>
       </c>
       <c r="Y4" t="s">
-        <v>147</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.2">
@@ -1418,7 +1442,7 @@
         <v>96</v>
       </c>
       <c r="Y5" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Phase-2 Start Add Interaction Comment Check.
</commit_message>
<xml_diff>
--- a/Excels/KE.xlsx
+++ b/Excels/KE.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="167">
   <si>
     <t>loginAuuid</t>
   </si>
@@ -517,6 +517,30 @@
   </si>
   <si>
     <t>240720001011</t>
+  </si>
+  <si>
+    <t>270720001022</t>
+  </si>
+  <si>
+    <t>270720001023</t>
+  </si>
+  <si>
+    <t>270720001024</t>
+  </si>
+  <si>
+    <t>270720001025</t>
+  </si>
+  <si>
+    <t>270720001027</t>
+  </si>
+  <si>
+    <t>270720001028</t>
+  </si>
+  <si>
+    <t>270720001029</t>
+  </si>
+  <si>
+    <t>270720001030</t>
   </si>
 </sst>
 </file>
@@ -1301,7 +1325,7 @@
         <v>96</v>
       </c>
       <c r="Y2" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.2">
@@ -1348,7 +1372,7 @@
         <v>96</v>
       </c>
       <c r="Y3" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.2">
@@ -1395,7 +1419,7 @@
         <v>96</v>
       </c>
       <c r="Y4" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.2">
@@ -1442,7 +1466,7 @@
         <v>96</v>
       </c>
       <c r="Y5" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Phase 2 And API Integration
Signed-off-by: Ravtej Singh <a_ravtej.singh@africa.airtel.com>
</commit_message>
<xml_diff>
--- a/Excels/KE.xlsx
+++ b/Excels/KE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a2388006/git/CS_PORTAL/Excels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B51DC590-8B83-D742-81F7-6D7629AB4F8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C54FF998-F242-DC4D-9B0F-4CAD6CACCBCB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20280" xr2:uid="{1FFDF3F0-6759-694F-9CB5-F32127F0BD7D}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="148">
   <si>
     <t>loginAuuid</t>
   </si>
@@ -463,6 +463,27 @@
   </si>
   <si>
     <t>API</t>
+  </si>
+  <si>
+    <t>string string string</t>
+  </si>
+  <si>
+    <t>National ID</t>
+  </si>
+  <si>
+    <t>***22222</t>
+  </si>
+  <si>
+    <t>8925403522001884647</t>
+  </si>
+  <si>
+    <t>01: 17 AM</t>
+  </si>
+  <si>
+    <t>28 May 2020</t>
+  </si>
+  <si>
+    <t>08-Jul-2020</t>
   </si>
 </sst>
 </file>
@@ -940,7 +961,7 @@
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1007,37 +1028,7 @@
         <v>131</v>
       </c>
       <c r="D2">
-        <v>735873718</v>
-      </c>
-      <c r="E2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K2">
-        <v>20772248</v>
-      </c>
-      <c r="L2">
-        <v>10441790</v>
-      </c>
-      <c r="M2" t="s">
-        <v>15</v>
-      </c>
-      <c r="N2" t="s">
-        <v>16</v>
+        <v>782945113</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
@@ -1050,6 +1041,39 @@
       <c r="C3" t="s">
         <v>130</v>
       </c>
+      <c r="D3">
+        <v>783425592</v>
+      </c>
+      <c r="E3" t="s">
+        <v>141</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="J3" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3">
+        <v>22418813</v>
+      </c>
+      <c r="L3">
+        <v>28905441</v>
+      </c>
+      <c r="M3" t="s">
+        <v>142</v>
+      </c>
+      <c r="N3" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4">
@@ -1060,6 +1084,39 @@
       </c>
       <c r="C4" t="s">
         <v>140</v>
+      </c>
+      <c r="D4">
+        <v>735873718</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K4">
+        <v>20772248</v>
+      </c>
+      <c r="L4">
+        <v>10441790</v>
+      </c>
+      <c r="M4" t="s">
+        <v>15</v>
+      </c>
+      <c r="N4" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1068,6 +1125,7 @@
     <hyperlink ref="B3" r:id="rId2" xr:uid="{033D127A-F434-CE46-9548-8CBA06150182}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Phase-2 Validate Ticket Escalation & Filter
</commit_message>
<xml_diff>
--- a/Excels/KE.xlsx
+++ b/Excels/KE.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a2388006/git/CS_PORTAL/Excels/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2394650\IdeaProjects\cs-portal-automation_selenium1\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17467F3A-4C0A-7549-A87B-F7AA9C1F7E3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20280" activeTab="1" xr2:uid="{1FFDF3F0-6759-694F-9CB5-F32127F0BD7D}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="35835" windowHeight="20280"/>
   </bookViews>
   <sheets>
     <sheet name="LoginCredentials" sheetId="1" r:id="rId1"/>
@@ -22,7 +21,7 @@
     <sheet name="InteractionChannel" sheetId="4" r:id="rId7"/>
     <sheet name="Ticket State" sheetId="6" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="145">
   <si>
     <t>loginAuuid</t>
   </si>
@@ -393,9 +392,6 @@
     <t>Social media</t>
   </si>
   <si>
-    <t>Secure@2024</t>
-  </si>
-  <si>
     <t>Tag Name</t>
   </si>
   <si>
@@ -453,84 +449,6 @@
     <t xml:space="preserve">Noise on Call </t>
   </si>
   <si>
-    <t>220720000981</t>
-  </si>
-  <si>
-    <t>220720000982</t>
-  </si>
-  <si>
-    <t>220720000983</t>
-  </si>
-  <si>
-    <t>220720000984</t>
-  </si>
-  <si>
-    <t>220720000986</t>
-  </si>
-  <si>
-    <t>220720000987</t>
-  </si>
-  <si>
-    <t>220720000988</t>
-  </si>
-  <si>
-    <t>220720000989</t>
-  </si>
-  <si>
-    <t>230720001051</t>
-  </si>
-  <si>
-    <t>230720001052</t>
-  </si>
-  <si>
-    <t>230720001053</t>
-  </si>
-  <si>
-    <t>230720001054</t>
-  </si>
-  <si>
-    <t>230720001055</t>
-  </si>
-  <si>
-    <t>230720001056</t>
-  </si>
-  <si>
-    <t>240720001004</t>
-  </si>
-  <si>
-    <t>240720001005</t>
-  </si>
-  <si>
-    <t>240720001006</t>
-  </si>
-  <si>
-    <t>240720001007</t>
-  </si>
-  <si>
-    <t>240720001008</t>
-  </si>
-  <si>
-    <t>240720001009</t>
-  </si>
-  <si>
-    <t>240720001010</t>
-  </si>
-  <si>
-    <t>240720001011</t>
-  </si>
-  <si>
-    <t>270720001022</t>
-  </si>
-  <si>
-    <t>270720001023</t>
-  </si>
-  <si>
-    <t>270720001024</t>
-  </si>
-  <si>
-    <t>270720001025</t>
-  </si>
-  <si>
     <t>270720001027</t>
   </si>
   <si>
@@ -541,12 +459,27 @@
   </si>
   <si>
     <t>270720001030</t>
+  </si>
+  <si>
+    <t>Jul@2020</t>
+  </si>
+  <si>
+    <t>280720001032</t>
+  </si>
+  <si>
+    <t>280720001033</t>
+  </si>
+  <si>
+    <t>280720001034</t>
+  </si>
+  <si>
+    <t>280720001035</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="0"/>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -1015,23 +948,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{365E7A5F-3E6A-E248-889F-23B3A6B34B5F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="17.1640625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="17.125" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="14.5" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="13.1640625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="13.125" collapsed="true"/>
     <col min="7" max="8" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="20.33203125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="20.375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1075,15 +1008,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2388006</v>
+        <v>2390932</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>117</v>
+        <v>140</v>
       </c>
       <c r="C2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D2">
         <v>735873718</v>
@@ -1119,62 +1052,62 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2394650</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C3" t="s">
         <v>131</v>
-      </c>
-      <c r="C3" t="s">
-        <v>132</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{E8376607-2FF2-6F45-92FA-BC7B676EA2F8}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{033D127A-F434-CE46-9548-8CBA06150182}"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ADE7D9A-20CD-0642-B0EB-506ABCE7F81B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="125" workbookViewId="0">
+    <sheetView topLeftCell="R1" zoomScale="125" workbookViewId="0">
       <selection activeCell="Y2" sqref="Y2:Y5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.83203125" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.875" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="3" max="4" bestFit="true" customWidth="true" width="23.83203125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="3" max="4" bestFit="true" customWidth="true" width="23.875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="18.625" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
     <col min="7" max="7" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="12.33203125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="12.375" collapsed="true"/>
     <col min="9" max="9" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
     <col min="10" max="10" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="12.33203125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="12.375" collapsed="true"/>
     <col min="12" max="12" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
     <col min="13" max="13" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="12.33203125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="12.375" collapsed="true"/>
     <col min="15" max="15" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
     <col min="16" max="16" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="12.33203125" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="12.375" collapsed="true"/>
     <col min="18" max="18" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
     <col min="19" max="19" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="12.33203125" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="23.83203125" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="12.375" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="23.875" collapsed="true"/>
     <col min="22" max="22" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="23.83203125" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="9.83203125" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="23.875" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="9.875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>40</v>
       </c>
@@ -1251,7 +1184,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>62</v>
       </c>
@@ -1325,10 +1258,10 @@
         <v>96</v>
       </c>
       <c r="Y2" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>62</v>
       </c>
@@ -1372,10 +1305,10 @@
         <v>96</v>
       </c>
       <c r="Y3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>62</v>
       </c>
@@ -1419,10 +1352,10 @@
         <v>96</v>
       </c>
       <c r="Y4" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>62</v>
       </c>
@@ -1466,7 +1399,7 @@
         <v>96</v>
       </c>
       <c r="Y5" t="s">
-        <v>166</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -1475,22 +1408,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA18D7CE-432C-7A43-A937-8C3A527B0618}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="186" workbookViewId="0">
       <selection activeCell="E7" sqref="A7:E117"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="11.5" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="28.6640625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="28.625" collapsed="true"/>
     <col min="3" max="4" bestFit="true" customWidth="true" width="24.5" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="18.625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>40</v>
       </c>
@@ -1507,7 +1440,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>22</v>
       </c>
@@ -1524,7 +1457,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>22</v>
       </c>
@@ -1541,7 +1474,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>28</v>
       </c>
@@ -1558,7 +1491,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>22</v>
       </c>
@@ -1575,7 +1508,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>28</v>
       </c>
@@ -1598,74 +1531,74 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ABC7933-64C1-7849-8110-0D430F2D9447}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>92</v>
       </c>
@@ -1676,106 +1609,106 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2075ED1E-EF94-2C4E-9A1E-007E8D0BAE3B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>92</v>
       </c>
@@ -1786,32 +1719,32 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E291AC0-838D-6744-8DB9-09A3DAD3E491}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>58</v>
@@ -1823,9 +1756,9 @@
         <v>735873718</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>58</v>
@@ -1837,9 +1770,9 @@
         <v>735873718</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>58</v>
@@ -1858,43 +1791,43 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87245F3F-7DE1-BD46-9DB5-A9FF4078DC57}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.1640625" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.125" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
-    <col min="3" max="4" bestFit="true" customWidth="true" width="28.33203125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="18.6640625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="17.1640625" collapsed="true"/>
+    <col min="3" max="4" bestFit="true" customWidth="true" width="28.375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="18.625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="17.125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>116</v>
       </c>
@@ -1905,7 +1838,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27323111-864D-DF45-AB3E-D4F27B17566B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
@@ -1915,62 +1848,62 @@
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="24.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="14.83203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="14.875" collapsed="true"/>
     <col min="3" max="3" customWidth="true" width="16.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>122</v>
       </c>
-      <c r="B2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>127</v>
-      </c>
-      <c r="B3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>126</v>
-      </c>
-      <c r="B4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>125</v>
-      </c>
-      <c r="B5" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>123</v>
-      </c>
       <c r="B6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C6" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
Phase-2 Validate the Option of Filter for Backend Supervisor and APPLY Filter         Agent can save or cancel the updated detail[Backend Agent]         Validate the Option of Filter for Backend Agent and APPLY Filter         Add new Comment[Backend Supervisor]         assignToAgentPOM Improve
</commit_message>
<xml_diff>
--- a/Excels/KE.xlsx
+++ b/Excels/KE.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="35835" windowHeight="20280"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="35835" windowHeight="20280" firstSheet="3" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="LoginCredentials" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="PinnedTags" sheetId="5" r:id="rId6"/>
     <sheet name="InteractionChannel" sheetId="4" r:id="rId7"/>
     <sheet name="Ticket State" sheetId="6" r:id="rId8"/>
+    <sheet name="Priority" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="155">
   <si>
     <t>loginAuuid</t>
   </si>
@@ -449,18 +450,6 @@
     <t xml:space="preserve">Noise on Call </t>
   </si>
   <si>
-    <t>270720001027</t>
-  </si>
-  <si>
-    <t>270720001028</t>
-  </si>
-  <si>
-    <t>270720001029</t>
-  </si>
-  <si>
-    <t>270720001030</t>
-  </si>
-  <si>
     <t>Jul@2020</t>
   </si>
   <si>
@@ -474,6 +463,48 @@
   </si>
   <si>
     <t>280720001035</t>
+  </si>
+  <si>
+    <t>Ticket Priority</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medium </t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Critical</t>
+  </si>
+  <si>
+    <t>Standard</t>
+  </si>
+  <si>
+    <t>Urgent</t>
+  </si>
+  <si>
+    <t>290720001037</t>
+  </si>
+  <si>
+    <t>290720001038</t>
+  </si>
+  <si>
+    <t>290720001039</t>
+  </si>
+  <si>
+    <t>290720001040</t>
+  </si>
+  <si>
+    <t>290720001042</t>
+  </si>
+  <si>
+    <t>290720001043</t>
+  </si>
+  <si>
+    <t>290720001044</t>
   </si>
 </sst>
 </file>
@@ -525,7 +556,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -547,6 +578,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -618,7 +655,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -634,6 +671,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -951,7 +989,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -1013,7 +1051,7 @@
         <v>2390932</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C2" t="s">
         <v>132</v>
@@ -1076,7 +1114,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y5"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" zoomScale="125" workbookViewId="0">
+    <sheetView topLeftCell="R7" zoomScale="125" workbookViewId="0">
       <selection activeCell="Y2" sqref="Y2:Y5"/>
     </sheetView>
   </sheetViews>
@@ -1258,7 +1296,7 @@
         <v>96</v>
       </c>
       <c r="Y2" t="s">
-        <v>141</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -1305,7 +1343,7 @@
         <v>96</v>
       </c>
       <c r="Y3" t="s">
-        <v>142</v>
+        <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
@@ -1352,7 +1390,7 @@
         <v>96</v>
       </c>
       <c r="Y4" t="s">
-        <v>143</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -1399,7 +1437,7 @@
         <v>96</v>
       </c>
       <c r="Y5" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -1913,4 +1951,57 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="16.5" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>147</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Phase-2 Add Frontend Agent Flow-InProgress
</commit_message>
<xml_diff>
--- a/Excels/KE.xlsx
+++ b/Excels/KE.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2394650\IdeaProjects\cs-portal-automation_selenium1\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="35835" windowHeight="20280" firstSheet="3" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="35835" windowHeight="20280"/>
   </bookViews>
   <sheets>
     <sheet name="LoginCredentials" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="148">
   <si>
     <t>loginAuuid</t>
   </si>
@@ -432,9 +432,6 @@
     <t>Ticket State Name</t>
   </si>
   <si>
-    <t>July@123</t>
-  </si>
-  <si>
     <t>BA</t>
   </si>
   <si>
@@ -450,21 +447,6 @@
     <t xml:space="preserve">Noise on Call </t>
   </si>
   <si>
-    <t>Jul@2020</t>
-  </si>
-  <si>
-    <t>280720001032</t>
-  </si>
-  <si>
-    <t>280720001033</t>
-  </si>
-  <si>
-    <t>280720001034</t>
-  </si>
-  <si>
-    <t>280720001035</t>
-  </si>
-  <si>
     <t>Ticket Priority</t>
   </si>
   <si>
@@ -486,15 +468,6 @@
     <t>Urgent</t>
   </si>
   <si>
-    <t>290720001037</t>
-  </si>
-  <si>
-    <t>290720001038</t>
-  </si>
-  <si>
-    <t>290720001039</t>
-  </si>
-  <si>
     <t>290720001040</t>
   </si>
   <si>
@@ -505,13 +478,18 @@
   </si>
   <si>
     <t>290720001044</t>
+  </si>
+  <si>
+    <t>July@123$</t>
+  </si>
+  <si>
+    <t>secure#321</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -989,17 +967,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="17.125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="14.5" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="13.125" collapsed="true"/>
-    <col min="7" max="8" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="20.375" collapsed="true"/>
+    <col min="4" max="4" width="17.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="20.375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -1048,13 +1026,13 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2390932</v>
+        <v>2388192</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>136</v>
+        <v>147</v>
       </c>
       <c r="C2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D2">
         <v>735873718</v>
@@ -1092,18 +1070,18 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2394650</v>
+        <v>2390495</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C3" t="s">
         <v>130</v>
-      </c>
-      <c r="C3" t="s">
-        <v>131</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId1" display="Jul@2020"/>
     <hyperlink ref="B3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1120,29 +1098,29 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="3" max="4" bestFit="true" customWidth="true" width="23.875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="18.625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="12.375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="12.375" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="12.375" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="12.375" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="12.375" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="23.875" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="23.875" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="9.875" collapsed="true"/>
+    <col min="1" max="1" width="11.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="23.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="17.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="17.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="17.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="17.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="23.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="17.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="23.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="9.875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1296,7 +1274,7 @@
         <v>96</v>
       </c>
       <c r="Y2" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -1343,7 +1321,7 @@
         <v>96</v>
       </c>
       <c r="Y3" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
@@ -1390,7 +1368,7 @@
         <v>96</v>
       </c>
       <c r="Y4" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -1437,7 +1415,7 @@
         <v>96</v>
       </c>
       <c r="Y5" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -1455,10 +1433,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.5" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="28.625" collapsed="true"/>
-    <col min="3" max="4" bestFit="true" customWidth="true" width="24.5" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="18.625" collapsed="true"/>
+    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="28.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="24.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1578,7 +1556,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="1" max="1" width="22" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1782,7 +1760,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>58</v>
@@ -1796,7 +1774,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>58</v>
@@ -1810,7 +1788,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>58</v>
@@ -1830,7 +1808,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:C26"/>
@@ -1838,11 +1816,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
-    <col min="3" max="4" bestFit="true" customWidth="true" width="28.375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="18.625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="17.125" collapsed="true"/>
+    <col min="1" max="1" width="14.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="28.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -1888,9 +1866,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="24.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="14.875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="1" max="1" width="24" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1957,48 +1935,48 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.5" collapsed="true"/>
+    <col min="1" max="1" width="16.5" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Phase-2 Add Frontend Agent Flow-Complete
</commit_message>
<xml_diff>
--- a/Excels/KE.xlsx
+++ b/Excels/KE.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2394650\IdeaProjects\cs-portal-automation_selenium1\Excels\"/>
     </mc:Choice>
@@ -24,7 +24,7 @@
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="155">
   <si>
     <t>loginAuuid</t>
   </si>
@@ -484,12 +484,34 @@
   </si>
   <si>
     <t>secure#321</t>
+  </si>
+  <si>
+    <t>040820001131</t>
+  </si>
+  <si>
+    <t>040820001132</t>
+  </si>
+  <si>
+    <t>040820001133</t>
+  </si>
+  <si>
+    <t>040820001134</t>
+  </si>
+  <si>
+    <t>040820001136</t>
+  </si>
+  <si>
+    <t>040820001137</t>
+  </si>
+  <si>
+    <t>040820001138</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -973,11 +995,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="17.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="8" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="20.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="17.125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="14.5" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="13.125" collapsed="true"/>
+    <col min="7" max="8" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="20.375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -1098,29 +1120,29 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="23.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18.625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="17.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="17.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="17.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="17.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="17.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="23.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="17.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="23.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="9.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="3" max="4" bestFit="true" customWidth="true" width="23.875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="18.625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="12.375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="12.375" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="12.375" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="12.375" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="12.375" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="23.875" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="23.875" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="9.875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1274,7 +1296,7 @@
         <v>96</v>
       </c>
       <c r="Y2" t="s">
-        <v>143</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -1321,7 +1343,7 @@
         <v>96</v>
       </c>
       <c r="Y3" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
@@ -1368,7 +1390,7 @@
         <v>96</v>
       </c>
       <c r="Y4" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -1415,7 +1437,7 @@
         <v>96</v>
       </c>
       <c r="Y5" t="s">
-        <v>142</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -1433,10 +1455,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="28.625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="24.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.5" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="28.625" collapsed="true"/>
+    <col min="3" max="4" bestFit="true" customWidth="true" width="24.5" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="18.625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1556,7 +1578,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1808,7 +1830,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:C26"/>
@@ -1816,11 +1838,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="28.375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18.625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="17.125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
+    <col min="3" max="4" bestFit="true" customWidth="true" width="28.375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="18.625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="17.125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -1866,9 +1888,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="24.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="14.875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="16.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1941,7 +1963,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="16.5" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Adding Header And error Handling To DashBoard
Signed-off-by: Ravtej Singh <a_ravtej.singh@africa.airtel.com>
</commit_message>
<xml_diff>
--- a/Excels/KE.xlsx
+++ b/Excels/KE.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a2388006/git/CS_PORTAL/Excels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73966AA0-A4BE-6D41-BE6D-38D10976BE3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB782F74-667C-AE48-920A-327F301962FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20280" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginCredentials" sheetId="1" r:id="rId1"/>
-    <sheet name="NFTRTickets" sheetId="3" r:id="rId2"/>
-    <sheet name="FTRTickets" sheetId="2" r:id="rId3"/>
-    <sheet name="WorkFlows" sheetId="7" r:id="rId4"/>
-    <sheet name="LoginQueue" sheetId="8" r:id="rId5"/>
-    <sheet name="PinnedTags" sheetId="5" r:id="rId6"/>
-    <sheet name="InteractionChannel" sheetId="4" r:id="rId7"/>
-    <sheet name="Ticket State" sheetId="6" r:id="rId8"/>
+    <sheet name="Headers" sheetId="9" r:id="rId2"/>
+    <sheet name="NFTRTickets" sheetId="3" r:id="rId3"/>
+    <sheet name="FTRTickets" sheetId="2" r:id="rId4"/>
+    <sheet name="WorkFlows" sheetId="7" r:id="rId5"/>
+    <sheet name="LoginQueue" sheetId="8" r:id="rId6"/>
+    <sheet name="PinnedTags" sheetId="5" r:id="rId7"/>
+    <sheet name="InteractionChannel" sheetId="4" r:id="rId8"/>
+    <sheet name="Ticket State" sheetId="6" r:id="rId9"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="187">
   <si>
     <t>loginAuuid</t>
   </si>
@@ -464,13 +465,143 @@
   </si>
   <si>
     <t>Field 6 Type</t>
+  </si>
+  <si>
+    <t>TableName</t>
+  </si>
+  <si>
+    <t>Row1</t>
+  </si>
+  <si>
+    <t>Row2</t>
+  </si>
+  <si>
+    <t>Row3</t>
+  </si>
+  <si>
+    <t>Row4</t>
+  </si>
+  <si>
+    <t>Row5</t>
+  </si>
+  <si>
+    <t>Row6</t>
+  </si>
+  <si>
+    <t>Row7</t>
+  </si>
+  <si>
+    <t>Amount (Ksh)</t>
+  </si>
+  <si>
+    <t>To/From</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Txn ID</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Usage History</t>
+  </si>
+  <si>
+    <t>Charges</t>
+  </si>
+  <si>
+    <t>Date &amp; Time</t>
+  </si>
+  <si>
+    <t>Start Balance</t>
+  </si>
+  <si>
+    <t>End Balance</t>
+  </si>
+  <si>
+    <t>Charges (Ksh)</t>
+  </si>
+  <si>
+    <t>Bundle Name</t>
+  </si>
+  <si>
+    <t>Recharge History</t>
+  </si>
+  <si>
+    <t>Benefit
+Voice|Data|SMS</t>
+  </si>
+  <si>
+    <t>Package Category</t>
+  </si>
+  <si>
+    <t>Transaction Number</t>
+  </si>
+  <si>
+    <t>Subscription Date &amp; Time</t>
+  </si>
+  <si>
+    <t>Expires On</t>
+  </si>
+  <si>
+    <t>Validity</t>
+  </si>
+  <si>
+    <t>Bundle Price (Ksh)</t>
+  </si>
+  <si>
+    <t>SMS To</t>
+  </si>
+  <si>
+    <t>Used Data</t>
+  </si>
+  <si>
+    <t>Call Duration</t>
+  </si>
+  <si>
+    <t>Call To</t>
+  </si>
+  <si>
+    <t>Row8</t>
+  </si>
+  <si>
+    <t>DA Id</t>
+  </si>
+  <si>
+    <t>DA Description</t>
+  </si>
+  <si>
+    <t>Bundle Type</t>
+  </si>
+  <si>
+    <t>Current DA Balance</t>
+  </si>
+  <si>
+    <t>Expiry Date</t>
+  </si>
+  <si>
+    <t>Bundle Subscription History</t>
+  </si>
+  <si>
+    <t>SMS History</t>
+  </si>
+  <si>
+    <t>Data History</t>
+  </si>
+  <si>
+    <t>Call History</t>
+  </si>
+  <si>
+    <t>Da Details</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -509,6 +640,12 @@
       <u/>
       <sz val="12"/>
       <color rgb="FF0066CC"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -638,6 +775,59 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9217" name="AutoShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{954E16FB-6A94-A343-90CA-E894AD77BEF0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="1841500"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -939,8 +1129,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -998,10 +1188,10 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>2394650</v>
+        <v>2388006</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="C2" t="s">
         <v>128</v>
@@ -1042,10 +1232,10 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>2388006</v>
+        <v>2394650</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="C3" t="s">
         <v>127</v>
@@ -1104,6 +1294,250 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5957FE73-F683-F440-8166-0945AED3D9E0}">
+  <dimension ref="A1:I9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L33" sqref="L33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AB5"/>
   <sheetViews>
@@ -1459,7 +1893,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
@@ -1582,7 +2016,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:A12"/>
   <sheetViews>
@@ -1660,7 +2094,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:A19"/>
   <sheetViews>
@@ -1770,7 +2204,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
@@ -1842,7 +2276,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
@@ -1889,7 +2323,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <tabColor theme="7"/>

</xml_diff>

<commit_message>
Workgroup Added and locator changed
</commit_message>
<xml_diff>
--- a/Excels/KE.xlsx
+++ b/Excels/KE.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3755" uniqueCount="1028">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3752" uniqueCount="1025">
   <si>
     <t>loginAuuid</t>
   </si>
@@ -2717,15 +2717,6 @@
   </si>
   <si>
     <t>200920001413</t>
-  </si>
-  <si>
-    <t>200920001414</t>
-  </si>
-  <si>
-    <t>200920001415</t>
-  </si>
-  <si>
-    <t>200920001416</t>
   </si>
   <si>
     <t>200920001418</t>
@@ -3585,7 +3576,7 @@
         <xdr:cNvPr id="9217" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{954E16FB-6A94-A343-90CA-E894AD77BEF0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{954E16FB-6A94-A343-90CA-E894AD77BEF0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4389,19 +4380,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>994</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>995</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>996</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>997</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>998</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>999</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1000</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>1001</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -4409,10 +4400,10 @@
         <v>634</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1003</v>
+        <v>1000</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>91</v>
@@ -4426,16 +4417,16 @@
         <v>634</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1004</v>
+        <v>1001</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>91</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>1005</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -4443,10 +4434,10 @@
         <v>636</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1003</v>
+        <v>1000</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>88</v>
@@ -4460,10 +4451,10 @@
         <v>636</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1006</v>
+        <v>1003</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>88</v>
@@ -4477,16 +4468,16 @@
         <v>723</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>81</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>1008</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -4494,16 +4485,16 @@
         <v>723</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1009</v>
+        <v>1006</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>81</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>1010</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -4511,16 +4502,16 @@
         <v>726</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>81</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>1008</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -4528,16 +4519,16 @@
         <v>726</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1009</v>
+        <v>1006</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>81</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>1010</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -4545,16 +4536,16 @@
         <v>729</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>81</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>1008</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -4562,16 +4553,16 @@
         <v>729</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1009</v>
+        <v>1006</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>81</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>1010</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -4579,16 +4570,16 @@
         <v>732</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>81</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>1008</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -4596,16 +4587,16 @@
         <v>732</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1009</v>
+        <v>1006</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>81</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>1010</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -4613,16 +4604,16 @@
         <v>735</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>81</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>1008</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -4630,16 +4621,16 @@
         <v>735</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>1009</v>
+        <v>1006</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>81</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>1010</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -4647,16 +4638,16 @@
         <v>738</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>81</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>1008</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -4664,16 +4655,16 @@
         <v>738</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1009</v>
+        <v>1006</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>81</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>1010</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -4681,16 +4672,16 @@
         <v>741</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>81</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>1008</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -4698,16 +4689,16 @@
         <v>741</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>1009</v>
+        <v>1006</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>81</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>1010</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -4715,16 +4706,16 @@
         <v>743</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>81</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>1008</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -4732,16 +4723,16 @@
         <v>743</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>1009</v>
+        <v>1006</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>81</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>1010</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -4749,16 +4740,16 @@
         <v>223</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>84</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>1008</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -4766,16 +4757,16 @@
         <v>223</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>1009</v>
+        <v>1006</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>84</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>1010</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -4783,7 +4774,7 @@
         <v>223</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>207</v>
@@ -4800,7 +4791,7 @@
         <v>223</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>208</v>
@@ -4817,16 +4808,16 @@
         <v>226</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>84</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>1008</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -4834,16 +4825,16 @@
         <v>226</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>1009</v>
+        <v>1006</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>84</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>1010</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -4851,7 +4842,7 @@
         <v>226</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>207</v>
@@ -4868,7 +4859,7 @@
         <v>226</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>208</v>
@@ -4885,16 +4876,16 @@
         <v>772</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>84</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>1008</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -4902,16 +4893,16 @@
         <v>772</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>1009</v>
+        <v>1006</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>84</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>1010</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -4919,7 +4910,7 @@
         <v>772</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>207</v>
@@ -4936,7 +4927,7 @@
         <v>772</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>208</v>
@@ -4953,16 +4944,16 @@
         <v>229</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>84</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>1008</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -4970,16 +4961,16 @@
         <v>229</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>1009</v>
+        <v>1006</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>84</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>1010</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -4987,7 +4978,7 @@
         <v>229</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>207</v>
@@ -5004,7 +4995,7 @@
         <v>229</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>208</v>
@@ -5021,16 +5012,16 @@
         <v>844</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>84</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>1008</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -5038,16 +5029,16 @@
         <v>844</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>1009</v>
+        <v>1006</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>84</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>1010</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -5055,7 +5046,7 @@
         <v>844</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>207</v>
@@ -5072,7 +5063,7 @@
         <v>844</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>208</v>
@@ -5089,16 +5080,16 @@
         <v>847</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>84</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>1008</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -5106,16 +5097,16 @@
         <v>847</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>1009</v>
+        <v>1006</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>84</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>1010</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -5123,7 +5114,7 @@
         <v>847</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>207</v>
@@ -5140,7 +5131,7 @@
         <v>847</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>208</v>
@@ -5157,16 +5148,16 @@
         <v>850</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>84</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>1008</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -5174,16 +5165,16 @@
         <v>850</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1009</v>
+        <v>1006</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>84</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>1010</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -5191,7 +5182,7 @@
         <v>850</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>207</v>
@@ -5208,7 +5199,7 @@
         <v>850</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>208</v>
@@ -5225,16 +5216,16 @@
         <v>852</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>84</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>1008</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -5242,16 +5233,16 @@
         <v>852</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1009</v>
+        <v>1006</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>84</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>1010</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -5259,7 +5250,7 @@
         <v>852</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>207</v>
@@ -5276,7 +5267,7 @@
         <v>852</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>208</v>
@@ -5293,7 +5284,7 @@
         <v>775</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>209</v>
@@ -5310,16 +5301,16 @@
         <v>800</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>1009</v>
+        <v>1006</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>91</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>1010</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -5327,16 +5318,16 @@
         <v>800</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>1004</v>
+        <v>1001</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>91</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>1005</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -5344,16 +5335,16 @@
         <v>812</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>1009</v>
+        <v>1006</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>91</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>1010</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -5361,16 +5352,16 @@
         <v>812</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>1011</v>
+        <v>1008</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>91</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>1012</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -5378,7 +5369,7 @@
         <v>812</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>207</v>
@@ -5392,44 +5383,44 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>1013</v>
+        <v>1010</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>84</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>1008</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>1013</v>
+        <v>1010</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>1009</v>
+        <v>1006</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>84</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>1010</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>1013</v>
+        <v>1010</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>207</v>
@@ -5443,10 +5434,10 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>1013</v>
+        <v>1010</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>208</v>
@@ -5460,44 +5451,44 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>1014</v>
+        <v>1011</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>84</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>1008</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>1014</v>
+        <v>1011</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>1009</v>
+        <v>1006</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>84</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>1010</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>1014</v>
+        <v>1011</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>207</v>
@@ -5511,10 +5502,10 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>1014</v>
+        <v>1011</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>208</v>
@@ -5528,44 +5519,44 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>1015</v>
+        <v>1012</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>84</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>1008</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>1015</v>
+        <v>1012</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>1009</v>
+        <v>1006</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>84</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>1010</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>1015</v>
+        <v>1012</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>207</v>
@@ -5579,10 +5570,10 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>1015</v>
+        <v>1012</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>208</v>
@@ -5596,44 +5587,44 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>1016</v>
+        <v>1013</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>84</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>1008</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>1016</v>
+        <v>1013</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>1009</v>
+        <v>1006</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>84</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>1010</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>1016</v>
+        <v>1013</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>207</v>
@@ -5647,10 +5638,10 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>1016</v>
+        <v>1013</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>208</v>
@@ -5664,44 +5655,44 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>1017</v>
+        <v>1014</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>84</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>1008</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>1017</v>
+        <v>1014</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>1009</v>
+        <v>1006</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>84</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>1010</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>1017</v>
+        <v>1014</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>207</v>
@@ -5715,10 +5706,10 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>1017</v>
+        <v>1014</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>208</v>
@@ -5732,44 +5723,44 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>1018</v>
+        <v>1015</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>84</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>1008</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>1018</v>
+        <v>1015</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>1009</v>
+        <v>1006</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>84</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>1010</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>1018</v>
+        <v>1015</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>207</v>
@@ -5783,10 +5774,10 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>1018</v>
+        <v>1015</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>208</v>
@@ -5800,44 +5791,44 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>1019</v>
+        <v>1016</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>84</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>1008</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>1019</v>
+        <v>1016</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>1009</v>
+        <v>1006</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>84</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>1010</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>1019</v>
+        <v>1016</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>207</v>
@@ -5851,10 +5842,10 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>1019</v>
+        <v>1016</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>208</v>
@@ -6173,7 +6164,7 @@
   <dimension ref="A1:AL168"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="Z1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AI11" sqref="AI11"/>
+      <selection activeCell="AE5" sqref="AE5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6291,25 +6282,25 @@
         <v>75</v>
       </c>
       <c r="AC1" s="26" t="s">
+        <v>1018</v>
+      </c>
+      <c r="AD1" s="26" t="s">
+        <v>1019</v>
+      </c>
+      <c r="AE1" s="26" t="s">
+        <v>1020</v>
+      </c>
+      <c r="AF1" s="26" t="s">
+        <v>1022</v>
+      </c>
+      <c r="AG1" s="26" t="s">
         <v>1021</v>
       </c>
-      <c r="AD1" s="26" t="s">
-        <v>1022</v>
-      </c>
-      <c r="AE1" s="26" t="s">
+      <c r="AH1" s="26" t="s">
         <v>1023</v>
       </c>
-      <c r="AF1" s="26" t="s">
-        <v>1025</v>
-      </c>
-      <c r="AG1" s="26" t="s">
+      <c r="AI1" s="45" t="s">
         <v>1024</v>
-      </c>
-      <c r="AH1" s="26" t="s">
-        <v>1026</v>
-      </c>
-      <c r="AI1" s="45" t="s">
-        <v>1027</v>
       </c>
       <c r="AJ1" t="s">
         <v>86</v>
@@ -6388,8 +6379,6 @@
       <c r="AB2">
         <v>3</v>
       </c>
-      <c r="AC2" s="34"/>
-      <c r="AD2" s="34"/>
       <c r="AE2" s="34"/>
       <c r="AF2" s="34"/>
       <c r="AG2" s="34"/>
@@ -6446,9 +6435,6 @@
       <c r="AK3" t="s">
         <v>89</v>
       </c>
-      <c r="AL3" t="s">
-        <v>885</v>
-      </c>
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -6488,9 +6474,6 @@
       <c r="AK4" t="s">
         <v>89</v>
       </c>
-      <c r="AL4" t="s">
-        <v>886</v>
-      </c>
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -6530,9 +6513,6 @@
       <c r="AK5" t="s">
         <v>89</v>
       </c>
-      <c r="AL5" t="s">
-        <v>887</v>
-      </c>
     </row>
     <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -6698,7 +6678,7 @@
         <v>244</v>
       </c>
       <c r="P9" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
       <c r="Q9" t="s">
         <v>243</v>
@@ -6707,7 +6687,7 @@
         <v>245</v>
       </c>
       <c r="S9" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
       <c r="T9" t="s">
         <v>54</v>
@@ -6791,7 +6771,7 @@
         <v>244</v>
       </c>
       <c r="P10" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
       <c r="Q10" t="s">
         <v>243</v>
@@ -6800,7 +6780,7 @@
         <v>245</v>
       </c>
       <c r="S10" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
       <c r="T10" t="s">
         <v>54</v>
@@ -6884,7 +6864,7 @@
         <v>244</v>
       </c>
       <c r="P11" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
       <c r="Q11" t="s">
         <v>243</v>
@@ -6893,7 +6873,7 @@
         <v>245</v>
       </c>
       <c r="S11" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
       <c r="T11" t="s">
         <v>54</v>
@@ -6977,7 +6957,7 @@
         <v>244</v>
       </c>
       <c r="P12" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
       <c r="Q12" t="s">
         <v>243</v>
@@ -6986,7 +6966,7 @@
         <v>245</v>
       </c>
       <c r="S12" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
       <c r="T12" t="s">
         <v>54</v>
@@ -8700,22 +8680,22 @@
         <v>75</v>
       </c>
       <c r="AC1" s="26" t="s">
+        <v>1018</v>
+      </c>
+      <c r="AD1" s="26" t="s">
+        <v>1019</v>
+      </c>
+      <c r="AE1" s="26" t="s">
+        <v>1020</v>
+      </c>
+      <c r="AF1" s="26" t="s">
+        <v>1022</v>
+      </c>
+      <c r="AG1" s="26" t="s">
         <v>1021</v>
       </c>
-      <c r="AD1" s="26" t="s">
-        <v>1022</v>
-      </c>
-      <c r="AE1" s="26" t="s">
+      <c r="AH1" s="26" t="s">
         <v>1023</v>
-      </c>
-      <c r="AF1" s="26" t="s">
-        <v>1025</v>
-      </c>
-      <c r="AG1" s="26" t="s">
-        <v>1024</v>
-      </c>
-      <c r="AH1" s="26" t="s">
-        <v>1026</v>
       </c>
       <c r="AI1" s="26" t="s">
         <v>86</v>
@@ -8807,7 +8787,7 @@
         <v>89</v>
       </c>
       <c r="AK2" s="1" t="s">
-        <v>888</v>
+        <v>885</v>
       </c>
     </row>
     <row r="3" spans="1:37" ht="38.25" x14ac:dyDescent="0.25">
@@ -8866,7 +8846,7 @@
         <v>89</v>
       </c>
       <c r="AK3" s="1" t="s">
-        <v>889</v>
+        <v>886</v>
       </c>
     </row>
     <row r="4" spans="1:37" ht="63.75" x14ac:dyDescent="0.25">
@@ -8955,7 +8935,7 @@
         <v>89</v>
       </c>
       <c r="AK4" s="1" t="s">
-        <v>890</v>
+        <v>887</v>
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
@@ -9038,7 +9018,7 @@
         <v>89</v>
       </c>
       <c r="AK5" s="1" t="s">
-        <v>891</v>
+        <v>888</v>
       </c>
     </row>
     <row r="6" spans="1:37" ht="51" x14ac:dyDescent="0.25">
@@ -9115,7 +9095,7 @@
         <v>89</v>
       </c>
       <c r="AK6" s="1" t="s">
-        <v>892</v>
+        <v>889</v>
       </c>
     </row>
     <row r="7" spans="1:37" ht="51" x14ac:dyDescent="0.25">
@@ -9192,7 +9172,7 @@
         <v>89</v>
       </c>
       <c r="AK7" s="1" t="s">
-        <v>893</v>
+        <v>890</v>
       </c>
     </row>
     <row r="8" spans="1:37" ht="51" x14ac:dyDescent="0.25">
@@ -9269,7 +9249,7 @@
         <v>89</v>
       </c>
       <c r="AK8" s="1" t="s">
-        <v>894</v>
+        <v>891</v>
       </c>
     </row>
     <row r="9" spans="1:37" ht="51" x14ac:dyDescent="0.25">
@@ -9346,7 +9326,7 @@
         <v>89</v>
       </c>
       <c r="AK9" s="1" t="s">
-        <v>895</v>
+        <v>892</v>
       </c>
     </row>
     <row r="10" spans="1:37" ht="51" x14ac:dyDescent="0.25">
@@ -9423,7 +9403,7 @@
         <v>89</v>
       </c>
       <c r="AK10" s="1" t="s">
-        <v>896</v>
+        <v>893</v>
       </c>
     </row>
     <row r="11" spans="1:37" ht="63.75" x14ac:dyDescent="0.25">
@@ -9500,7 +9480,7 @@
         <v>89</v>
       </c>
       <c r="AK11" s="1" t="s">
-        <v>897</v>
+        <v>894</v>
       </c>
     </row>
     <row r="12" spans="1:37" ht="51" x14ac:dyDescent="0.25">
@@ -9577,7 +9557,7 @@
         <v>89</v>
       </c>
       <c r="AK12" s="1" t="s">
-        <v>898</v>
+        <v>895</v>
       </c>
     </row>
     <row r="13" spans="1:37" ht="63.75" x14ac:dyDescent="0.25">
@@ -9660,7 +9640,7 @@
         <v>89</v>
       </c>
       <c r="AK13" s="1" t="s">
-        <v>899</v>
+        <v>896</v>
       </c>
     </row>
     <row r="14" spans="1:37" ht="38.25" x14ac:dyDescent="0.25">
@@ -9719,7 +9699,7 @@
         <v>89</v>
       </c>
       <c r="AK14" s="1" t="s">
-        <v>900</v>
+        <v>897</v>
       </c>
     </row>
     <row r="15" spans="1:37" ht="38.25" x14ac:dyDescent="0.25">
@@ -9778,7 +9758,7 @@
         <v>89</v>
       </c>
       <c r="AK15" s="1" t="s">
-        <v>901</v>
+        <v>898</v>
       </c>
     </row>
     <row r="16" spans="1:37" ht="38.25" x14ac:dyDescent="0.25">
@@ -9837,7 +9817,7 @@
         <v>89</v>
       </c>
       <c r="AK16" s="1" t="s">
-        <v>902</v>
+        <v>899</v>
       </c>
     </row>
     <row r="17" spans="1:37" ht="38.25" x14ac:dyDescent="0.25">
@@ -9896,7 +9876,7 @@
         <v>89</v>
       </c>
       <c r="AK17" s="1" t="s">
-        <v>903</v>
+        <v>900</v>
       </c>
     </row>
     <row r="18" spans="1:37" ht="38.25" x14ac:dyDescent="0.25">
@@ -9967,7 +9947,7 @@
         <v>89</v>
       </c>
       <c r="AK18" s="1" t="s">
-        <v>904</v>
+        <v>901</v>
       </c>
     </row>
     <row r="19" spans="1:37" ht="38.25" x14ac:dyDescent="0.25">
@@ -10026,7 +10006,7 @@
         <v>89</v>
       </c>
       <c r="AK19" s="1" t="s">
-        <v>905</v>
+        <v>902</v>
       </c>
     </row>
     <row r="20" spans="1:37" ht="38.25" x14ac:dyDescent="0.25">
@@ -10085,7 +10065,7 @@
         <v>89</v>
       </c>
       <c r="AK20" s="1" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
     </row>
     <row r="21" spans="1:37" ht="51" x14ac:dyDescent="0.25">
@@ -10144,7 +10124,7 @@
         <v>89</v>
       </c>
       <c r="AK21" s="1" t="s">
-        <v>907</v>
+        <v>904</v>
       </c>
     </row>
     <row r="22" spans="1:37" ht="51" x14ac:dyDescent="0.25">
@@ -10203,7 +10183,7 @@
         <v>89</v>
       </c>
       <c r="AK22" s="1" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
     </row>
     <row r="23" spans="1:37" ht="89.25" x14ac:dyDescent="0.25">
@@ -10268,7 +10248,7 @@
         <v>89</v>
       </c>
       <c r="AK23" s="1" t="s">
-        <v>909</v>
+        <v>906</v>
       </c>
     </row>
     <row r="24" spans="1:37" ht="51" x14ac:dyDescent="0.25">
@@ -10345,7 +10325,7 @@
         <v>89</v>
       </c>
       <c r="AK24" s="1" t="s">
-        <v>910</v>
+        <v>907</v>
       </c>
     </row>
     <row r="25" spans="1:37" ht="38.25" x14ac:dyDescent="0.25">
@@ -10509,7 +10489,7 @@
         <v>89</v>
       </c>
       <c r="AK26" s="1" t="s">
-        <v>911</v>
+        <v>908</v>
       </c>
     </row>
     <row r="27" spans="1:37" ht="63.75" x14ac:dyDescent="0.25">
@@ -10598,7 +10578,7 @@
         <v>89</v>
       </c>
       <c r="AK27" s="1" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
     </row>
     <row r="28" spans="1:37" ht="76.5" x14ac:dyDescent="0.25">
@@ -10831,7 +10811,7 @@
         <v>89</v>
       </c>
       <c r="AK30" s="1" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
     </row>
     <row r="31" spans="1:37" ht="76.5" x14ac:dyDescent="0.25">
@@ -10890,7 +10870,7 @@
         <v>89</v>
       </c>
       <c r="AK31" s="1" t="s">
-        <v>914</v>
+        <v>911</v>
       </c>
     </row>
     <row r="32" spans="1:37" ht="51" x14ac:dyDescent="0.25">
@@ -10973,7 +10953,7 @@
         <v>89</v>
       </c>
       <c r="AK32" s="1" t="s">
-        <v>915</v>
+        <v>912</v>
       </c>
     </row>
     <row r="33" spans="1:37" ht="51" x14ac:dyDescent="0.25">
@@ -11050,7 +11030,7 @@
         <v>89</v>
       </c>
       <c r="AK33" s="1" t="s">
-        <v>916</v>
+        <v>913</v>
       </c>
     </row>
     <row r="34" spans="1:37" ht="25.5" x14ac:dyDescent="0.25">
@@ -11127,7 +11107,7 @@
         <v>89</v>
       </c>
       <c r="AK34" s="1" t="s">
-        <v>917</v>
+        <v>914</v>
       </c>
     </row>
     <row r="35" spans="1:37" ht="25.5" x14ac:dyDescent="0.25">
@@ -11204,7 +11184,7 @@
         <v>89</v>
       </c>
       <c r="AK35" s="1" t="s">
-        <v>918</v>
+        <v>915</v>
       </c>
     </row>
     <row r="36" spans="1:37" ht="38.25" x14ac:dyDescent="0.25">
@@ -11263,7 +11243,7 @@
         <v>89</v>
       </c>
       <c r="AK36" s="1" t="s">
-        <v>919</v>
+        <v>916</v>
       </c>
     </row>
     <row r="37" spans="1:37" ht="63.75" x14ac:dyDescent="0.25">
@@ -11352,7 +11332,7 @@
         <v>89</v>
       </c>
       <c r="AK37" s="1" t="s">
-        <v>920</v>
+        <v>917</v>
       </c>
     </row>
     <row r="38" spans="1:37" ht="38.25" x14ac:dyDescent="0.25">
@@ -11417,7 +11397,7 @@
         <v>89</v>
       </c>
       <c r="AK38" s="1" t="s">
-        <v>921</v>
+        <v>918</v>
       </c>
     </row>
     <row r="39" spans="1:37" ht="51" x14ac:dyDescent="0.25">
@@ -11482,7 +11462,7 @@
         <v>89</v>
       </c>
       <c r="AK39" s="1" t="s">
-        <v>922</v>
+        <v>919</v>
       </c>
     </row>
     <row r="40" spans="1:37" ht="76.5" x14ac:dyDescent="0.25">
@@ -11553,7 +11533,7 @@
         <v>89</v>
       </c>
       <c r="AK40" s="1" t="s">
-        <v>923</v>
+        <v>920</v>
       </c>
     </row>
     <row r="41" spans="1:37" ht="38.25" x14ac:dyDescent="0.25">
@@ -11618,7 +11598,7 @@
         <v>89</v>
       </c>
       <c r="AK41" s="1" t="s">
-        <v>924</v>
+        <v>921</v>
       </c>
     </row>
     <row r="42" spans="1:37" ht="51" x14ac:dyDescent="0.25">
@@ -11683,7 +11663,7 @@
         <v>89</v>
       </c>
       <c r="AK42" s="1" t="s">
-        <v>925</v>
+        <v>922</v>
       </c>
     </row>
     <row r="43" spans="1:37" ht="127.5" x14ac:dyDescent="0.25">
@@ -11748,7 +11728,7 @@
         <v>89</v>
       </c>
       <c r="AK43" s="1" t="s">
-        <v>926</v>
+        <v>923</v>
       </c>
     </row>
     <row r="44" spans="1:37" ht="76.5" x14ac:dyDescent="0.25">
@@ -11813,7 +11793,7 @@
         <v>89</v>
       </c>
       <c r="AK44" s="1" t="s">
-        <v>927</v>
+        <v>924</v>
       </c>
     </row>
     <row r="45" spans="1:37" ht="102" x14ac:dyDescent="0.25">
@@ -11876,7 +11856,7 @@
         <v>89</v>
       </c>
       <c r="AK45" s="1" t="s">
-        <v>928</v>
+        <v>925</v>
       </c>
     </row>
     <row r="46" spans="1:37" ht="25.5" x14ac:dyDescent="0.25">
@@ -11953,7 +11933,7 @@
         <v>89</v>
       </c>
       <c r="AK46" s="1" t="s">
-        <v>929</v>
+        <v>926</v>
       </c>
     </row>
     <row r="47" spans="1:37" ht="38.25" x14ac:dyDescent="0.25">
@@ -12093,7 +12073,7 @@
         <v>89</v>
       </c>
       <c r="AK48" s="1" t="s">
-        <v>930</v>
+        <v>927</v>
       </c>
     </row>
     <row r="49" spans="1:37" ht="63.75" x14ac:dyDescent="0.25">
@@ -12170,7 +12150,7 @@
         <v>89</v>
       </c>
       <c r="AK49" s="1" t="s">
-        <v>931</v>
+        <v>928</v>
       </c>
     </row>
     <row r="50" spans="1:37" ht="76.5" x14ac:dyDescent="0.25">
@@ -12247,7 +12227,7 @@
         <v>89</v>
       </c>
       <c r="AK50" s="1" t="s">
-        <v>932</v>
+        <v>929</v>
       </c>
     </row>
     <row r="51" spans="1:37" ht="63.75" x14ac:dyDescent="0.25">
@@ -12324,7 +12304,7 @@
         <v>89</v>
       </c>
       <c r="AK51" s="1" t="s">
-        <v>933</v>
+        <v>930</v>
       </c>
     </row>
     <row r="52" spans="1:37" ht="63.75" x14ac:dyDescent="0.25">
@@ -12389,7 +12369,7 @@
         <v>89</v>
       </c>
       <c r="AK52" s="1" t="s">
-        <v>934</v>
+        <v>931</v>
       </c>
     </row>
     <row r="53" spans="1:37" ht="63.75" x14ac:dyDescent="0.25">
@@ -12460,7 +12440,7 @@
         <v>89</v>
       </c>
       <c r="AK53" s="1" t="s">
-        <v>935</v>
+        <v>932</v>
       </c>
     </row>
     <row r="54" spans="1:37" ht="76.5" x14ac:dyDescent="0.25">
@@ -12549,7 +12529,7 @@
         <v>89</v>
       </c>
       <c r="AK54" s="1" t="s">
-        <v>936</v>
+        <v>933</v>
       </c>
     </row>
     <row r="55" spans="1:37" ht="51" x14ac:dyDescent="0.25">
@@ -12608,7 +12588,7 @@
         <v>89</v>
       </c>
       <c r="AK55" s="1" t="s">
-        <v>937</v>
+        <v>934</v>
       </c>
     </row>
     <row r="56" spans="1:37" ht="89.25" x14ac:dyDescent="0.25">
@@ -12673,7 +12653,7 @@
         <v>89</v>
       </c>
       <c r="AK56" s="1" t="s">
-        <v>938</v>
+        <v>935</v>
       </c>
     </row>
     <row r="57" spans="1:37" ht="51" x14ac:dyDescent="0.25">
@@ -12738,7 +12718,7 @@
         <v>89</v>
       </c>
       <c r="AK57" s="1" t="s">
-        <v>939</v>
+        <v>936</v>
       </c>
     </row>
     <row r="58" spans="1:37" ht="38.25" x14ac:dyDescent="0.25">
@@ -12815,7 +12795,7 @@
         <v>89</v>
       </c>
       <c r="AK58" s="1" t="s">
-        <v>940</v>
+        <v>937</v>
       </c>
     </row>
     <row r="59" spans="1:37" ht="51" x14ac:dyDescent="0.25">
@@ -12892,7 +12872,7 @@
         <v>89</v>
       </c>
       <c r="AK59" s="1" t="s">
-        <v>941</v>
+        <v>938</v>
       </c>
     </row>
     <row r="60" spans="1:37" ht="63.75" x14ac:dyDescent="0.25">
@@ -12975,7 +12955,7 @@
         <v>89</v>
       </c>
       <c r="AK60" s="1" t="s">
-        <v>942</v>
+        <v>939</v>
       </c>
     </row>
     <row r="61" spans="1:37" ht="25.5" x14ac:dyDescent="0.25">
@@ -13058,7 +13038,7 @@
         <v>89</v>
       </c>
       <c r="AK61" s="1" t="s">
-        <v>943</v>
+        <v>940</v>
       </c>
     </row>
     <row r="62" spans="1:37" ht="38.25" x14ac:dyDescent="0.25">
@@ -13123,7 +13103,7 @@
         <v>89</v>
       </c>
       <c r="AK62" s="1" t="s">
-        <v>944</v>
+        <v>941</v>
       </c>
     </row>
     <row r="63" spans="1:37" ht="38.25" x14ac:dyDescent="0.25">
@@ -13188,7 +13168,7 @@
         <v>89</v>
       </c>
       <c r="AK63" s="1" t="s">
-        <v>945</v>
+        <v>942</v>
       </c>
     </row>
     <row r="64" spans="1:37" ht="38.25" x14ac:dyDescent="0.25">
@@ -13253,7 +13233,7 @@
         <v>89</v>
       </c>
       <c r="AK64" s="1" t="s">
-        <v>946</v>
+        <v>943</v>
       </c>
     </row>
     <row r="65" spans="1:37" ht="38.25" x14ac:dyDescent="0.25">
@@ -13318,7 +13298,7 @@
         <v>89</v>
       </c>
       <c r="AK65" s="1" t="s">
-        <v>947</v>
+        <v>944</v>
       </c>
     </row>
     <row r="66" spans="1:37" ht="51" x14ac:dyDescent="0.25">
@@ -13395,7 +13375,7 @@
         <v>89</v>
       </c>
       <c r="AK66" s="1" t="s">
-        <v>948</v>
+        <v>945</v>
       </c>
     </row>
     <row r="67" spans="1:37" ht="38.25" x14ac:dyDescent="0.25">
@@ -13466,7 +13446,7 @@
         <v>89</v>
       </c>
       <c r="AK67" s="1" t="s">
-        <v>949</v>
+        <v>946</v>
       </c>
     </row>
     <row r="68" spans="1:37" ht="38.25" x14ac:dyDescent="0.25">
@@ -13543,7 +13523,7 @@
         <v>89</v>
       </c>
       <c r="AK68" s="1" t="s">
-        <v>950</v>
+        <v>947</v>
       </c>
     </row>
     <row r="69" spans="1:37" ht="51" x14ac:dyDescent="0.25">
@@ -13608,7 +13588,7 @@
         <v>89</v>
       </c>
       <c r="AK69" s="1" t="s">
-        <v>951</v>
+        <v>948</v>
       </c>
     </row>
     <row r="70" spans="1:37" ht="51" x14ac:dyDescent="0.25">
@@ -13685,7 +13665,7 @@
         <v>89</v>
       </c>
       <c r="AK70" s="1" t="s">
-        <v>952</v>
+        <v>949</v>
       </c>
     </row>
     <row r="71" spans="1:37" ht="51" x14ac:dyDescent="0.25">
@@ -13762,7 +13742,7 @@
         <v>89</v>
       </c>
       <c r="AK71" s="1" t="s">
-        <v>953</v>
+        <v>950</v>
       </c>
     </row>
     <row r="72" spans="1:37" ht="51" x14ac:dyDescent="0.25">
@@ -13827,7 +13807,7 @@
         <v>89</v>
       </c>
       <c r="AK72" s="1" t="s">
-        <v>954</v>
+        <v>951</v>
       </c>
     </row>
     <row r="73" spans="1:37" ht="51" x14ac:dyDescent="0.25">
@@ -13898,7 +13878,7 @@
         <v>89</v>
       </c>
       <c r="AK73" s="1" t="s">
-        <v>955</v>
+        <v>952</v>
       </c>
     </row>
     <row r="74" spans="1:37" ht="63.75" x14ac:dyDescent="0.25">
@@ -13969,7 +13949,7 @@
         <v>89</v>
       </c>
       <c r="AK74" s="1" t="s">
-        <v>956</v>
+        <v>953</v>
       </c>
     </row>
     <row r="75" spans="1:37" ht="63.75" x14ac:dyDescent="0.25">
@@ -14046,7 +14026,7 @@
         <v>89</v>
       </c>
       <c r="AK75" s="1" t="s">
-        <v>957</v>
+        <v>954</v>
       </c>
     </row>
     <row r="76" spans="1:37" ht="63.75" x14ac:dyDescent="0.25">
@@ -14123,7 +14103,7 @@
         <v>89</v>
       </c>
       <c r="AK76" s="1" t="s">
-        <v>958</v>
+        <v>955</v>
       </c>
     </row>
     <row r="77" spans="1:37" ht="51" x14ac:dyDescent="0.25">
@@ -14188,7 +14168,7 @@
         <v>89</v>
       </c>
       <c r="AK77" s="1" t="s">
-        <v>959</v>
+        <v>956</v>
       </c>
     </row>
     <row r="78" spans="1:37" ht="25.5" x14ac:dyDescent="0.25">
@@ -14253,7 +14233,7 @@
         <v>89</v>
       </c>
       <c r="AK78" s="1" t="s">
-        <v>960</v>
+        <v>957</v>
       </c>
     </row>
     <row r="79" spans="1:37" ht="51" x14ac:dyDescent="0.25">
@@ -14318,7 +14298,7 @@
         <v>89</v>
       </c>
       <c r="AK79" s="1" t="s">
-        <v>961</v>
+        <v>958</v>
       </c>
     </row>
     <row r="80" spans="1:37" ht="51" x14ac:dyDescent="0.25">
@@ -14395,7 +14375,7 @@
         <v>89</v>
       </c>
       <c r="AK80" s="1" t="s">
-        <v>962</v>
+        <v>959</v>
       </c>
     </row>
     <row r="81" spans="1:37" ht="38.25" x14ac:dyDescent="0.25">
@@ -14454,7 +14434,7 @@
         <v>89</v>
       </c>
       <c r="AK81" s="1" t="s">
-        <v>963</v>
+        <v>960</v>
       </c>
     </row>
     <row r="82" spans="1:37" ht="51" x14ac:dyDescent="0.25">
@@ -14519,7 +14499,7 @@
         <v>89</v>
       </c>
       <c r="AK82" s="1" t="s">
-        <v>964</v>
+        <v>961</v>
       </c>
     </row>
     <row r="83" spans="1:37" ht="38.25" x14ac:dyDescent="0.25">
@@ -14590,7 +14570,7 @@
         <v>89</v>
       </c>
       <c r="AK83" s="1" t="s">
-        <v>965</v>
+        <v>962</v>
       </c>
     </row>
     <row r="84" spans="1:37" ht="38.25" x14ac:dyDescent="0.25">
@@ -14655,7 +14635,7 @@
         <v>89</v>
       </c>
       <c r="AK84" s="1" t="s">
-        <v>966</v>
+        <v>963</v>
       </c>
     </row>
     <row r="85" spans="1:37" ht="38.25" x14ac:dyDescent="0.25">
@@ -14714,7 +14694,7 @@
         <v>89</v>
       </c>
       <c r="AK85" s="1" t="s">
-        <v>967</v>
+        <v>964</v>
       </c>
     </row>
     <row r="86" spans="1:37" ht="63.75" x14ac:dyDescent="0.25">
@@ -14953,7 +14933,7 @@
         <v>89</v>
       </c>
       <c r="AK88" s="1" t="s">
-        <v>968</v>
+        <v>965</v>
       </c>
     </row>
     <row r="89" spans="1:37" x14ac:dyDescent="0.25">
@@ -15030,7 +15010,7 @@
         <v>89</v>
       </c>
       <c r="AK89" s="1" t="s">
-        <v>969</v>
+        <v>966</v>
       </c>
     </row>
     <row r="90" spans="1:37" ht="89.25" x14ac:dyDescent="0.25">
@@ -15119,7 +15099,7 @@
         <v>89</v>
       </c>
       <c r="AK90" s="1" t="s">
-        <v>970</v>
+        <v>967</v>
       </c>
     </row>
     <row r="91" spans="1:37" ht="51" x14ac:dyDescent="0.25">
@@ -15184,7 +15164,7 @@
         <v>89</v>
       </c>
       <c r="AK91" s="1" t="s">
-        <v>971</v>
+        <v>968</v>
       </c>
     </row>
     <row r="92" spans="1:37" ht="51" x14ac:dyDescent="0.25">
@@ -15249,7 +15229,7 @@
         <v>89</v>
       </c>
       <c r="AK92" s="1" t="s">
-        <v>972</v>
+        <v>969</v>
       </c>
     </row>
     <row r="93" spans="1:37" ht="51" x14ac:dyDescent="0.25">
@@ -15314,7 +15294,7 @@
         <v>89</v>
       </c>
       <c r="AK93" s="1" t="s">
-        <v>973</v>
+        <v>970</v>
       </c>
     </row>
     <row r="94" spans="1:37" ht="51" x14ac:dyDescent="0.25">
@@ -15379,7 +15359,7 @@
         <v>89</v>
       </c>
       <c r="AK94" s="1" t="s">
-        <v>974</v>
+        <v>971</v>
       </c>
     </row>
     <row r="95" spans="1:37" ht="51" x14ac:dyDescent="0.25">
@@ -15444,7 +15424,7 @@
         <v>89</v>
       </c>
       <c r="AK95" s="1" t="s">
-        <v>975</v>
+        <v>972</v>
       </c>
     </row>
     <row r="96" spans="1:37" ht="102" x14ac:dyDescent="0.25">
@@ -15509,7 +15489,7 @@
         <v>89</v>
       </c>
       <c r="AK96" s="1" t="s">
-        <v>976</v>
+        <v>973</v>
       </c>
     </row>
     <row r="97" spans="1:37" ht="38.25" x14ac:dyDescent="0.25">
@@ -15586,7 +15566,7 @@
         <v>89</v>
       </c>
       <c r="AK97" s="1" t="s">
-        <v>977</v>
+        <v>974</v>
       </c>
     </row>
     <row r="98" spans="1:37" ht="38.25" x14ac:dyDescent="0.25">
@@ -15663,7 +15643,7 @@
         <v>89</v>
       </c>
       <c r="AK98" s="1" t="s">
-        <v>978</v>
+        <v>975</v>
       </c>
     </row>
     <row r="99" spans="1:37" ht="63.75" x14ac:dyDescent="0.25">
@@ -15740,7 +15720,7 @@
         <v>89</v>
       </c>
       <c r="AK99" s="1" t="s">
-        <v>979</v>
+        <v>976</v>
       </c>
     </row>
     <row r="100" spans="1:37" ht="25.5" x14ac:dyDescent="0.25">
@@ -15817,7 +15797,7 @@
         <v>89</v>
       </c>
       <c r="AK100" s="1" t="s">
-        <v>980</v>
+        <v>977</v>
       </c>
     </row>
     <row r="101" spans="1:37" ht="63.75" x14ac:dyDescent="0.25">
@@ -15894,7 +15874,7 @@
         <v>89</v>
       </c>
       <c r="AK101" s="1" t="s">
-        <v>981</v>
+        <v>978</v>
       </c>
     </row>
     <row r="102" spans="1:37" ht="89.25" x14ac:dyDescent="0.25">
@@ -15983,7 +15963,7 @@
         <v>89</v>
       </c>
       <c r="AK102" s="1" t="s">
-        <v>982</v>
+        <v>979</v>
       </c>
     </row>
     <row r="103" spans="1:37" ht="25.5" x14ac:dyDescent="0.25">
@@ -16048,7 +16028,7 @@
         <v>89</v>
       </c>
       <c r="AK103" s="1" t="s">
-        <v>983</v>
+        <v>980</v>
       </c>
     </row>
     <row r="104" spans="1:37" ht="63.75" x14ac:dyDescent="0.25">
@@ -16125,7 +16105,7 @@
         <v>89</v>
       </c>
       <c r="AK104" s="1" t="s">
-        <v>984</v>
+        <v>981</v>
       </c>
     </row>
     <row r="105" spans="1:37" ht="63.75" x14ac:dyDescent="0.25">
@@ -16202,7 +16182,7 @@
         <v>89</v>
       </c>
       <c r="AK105" s="1" t="s">
-        <v>985</v>
+        <v>982</v>
       </c>
     </row>
     <row r="106" spans="1:37" ht="51" x14ac:dyDescent="0.25">
@@ -16279,7 +16259,7 @@
         <v>89</v>
       </c>
       <c r="AK106" s="1" t="s">
-        <v>986</v>
+        <v>983</v>
       </c>
     </row>
     <row r="107" spans="1:37" ht="38.25" x14ac:dyDescent="0.25">
@@ -16362,7 +16342,7 @@
         <v>89</v>
       </c>
       <c r="AK107" s="1" t="s">
-        <v>987</v>
+        <v>984</v>
       </c>
     </row>
     <row r="108" spans="1:37" ht="63.75" x14ac:dyDescent="0.25">
@@ -16427,7 +16407,7 @@
         <v>89</v>
       </c>
       <c r="AK108" s="1" t="s">
-        <v>988</v>
+        <v>985</v>
       </c>
     </row>
     <row r="109" spans="1:37" ht="76.5" x14ac:dyDescent="0.25">
@@ -16492,7 +16472,7 @@
         <v>89</v>
       </c>
       <c r="AK109" s="1" t="s">
-        <v>989</v>
+        <v>986</v>
       </c>
     </row>
     <row r="110" spans="1:37" ht="51" x14ac:dyDescent="0.25">
@@ -16557,7 +16537,7 @@
         <v>89</v>
       </c>
       <c r="AK110" s="1" t="s">
-        <v>990</v>
+        <v>987</v>
       </c>
     </row>
     <row r="111" spans="1:37" ht="25.5" x14ac:dyDescent="0.25">
@@ -16616,7 +16596,7 @@
         <v>89</v>
       </c>
       <c r="AK111" s="1" t="s">
-        <v>991</v>
+        <v>988</v>
       </c>
     </row>
     <row r="112" spans="1:37" ht="25.5" x14ac:dyDescent="0.25">
@@ -16675,7 +16655,7 @@
         <v>89</v>
       </c>
       <c r="AK112" s="1" t="s">
-        <v>992</v>
+        <v>989</v>
       </c>
     </row>
     <row r="113" spans="1:37" ht="25.5" x14ac:dyDescent="0.25">
@@ -16734,7 +16714,7 @@
         <v>89</v>
       </c>
       <c r="AK113" s="1" t="s">
-        <v>993</v>
+        <v>990</v>
       </c>
     </row>
     <row r="114" spans="1:37" ht="25.5" x14ac:dyDescent="0.25">
@@ -16793,7 +16773,7 @@
         <v>89</v>
       </c>
       <c r="AK114" s="1" t="s">
-        <v>994</v>
+        <v>991</v>
       </c>
     </row>
     <row r="115" spans="1:37" ht="25.5" x14ac:dyDescent="0.25">
@@ -16852,7 +16832,7 @@
         <v>89</v>
       </c>
       <c r="AK115" s="1" t="s">
-        <v>995</v>
+        <v>992</v>
       </c>
     </row>
     <row r="116" spans="1:37" ht="25.5" x14ac:dyDescent="0.25">
@@ -16911,7 +16891,7 @@
         <v>89</v>
       </c>
       <c r="AK116" s="1" t="s">
-        <v>996</v>
+        <v>993</v>
       </c>
     </row>
     <row r="117" spans="1:37" x14ac:dyDescent="0.25">
@@ -16961,7 +16941,7 @@
         <v>244</v>
       </c>
       <c r="P117" s="13" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
       <c r="Q117" s="13" t="s">
         <v>243</v>
@@ -16970,7 +16950,7 @@
         <v>245</v>
       </c>
       <c r="S117" s="13" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
       <c r="T117" s="13" t="s">
         <v>54</v>
@@ -17060,7 +17040,7 @@
         <v>244</v>
       </c>
       <c r="P118" s="13" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
       <c r="Q118" s="13" t="s">
         <v>243</v>
@@ -17069,7 +17049,7 @@
         <v>245</v>
       </c>
       <c r="S118" s="13" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
       <c r="T118" s="13" t="s">
         <v>54</v>
@@ -17159,7 +17139,7 @@
         <v>244</v>
       </c>
       <c r="P119" s="13" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
       <c r="Q119" s="13" t="s">
         <v>243</v>
@@ -17168,7 +17148,7 @@
         <v>245</v>
       </c>
       <c r="S119" s="13" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
       <c r="T119" s="13" t="s">
         <v>54</v>
@@ -17252,7 +17232,7 @@
         <v>244</v>
       </c>
       <c r="P120" s="13" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
       <c r="Q120" s="13" t="s">
         <v>243</v>
@@ -17261,7 +17241,7 @@
         <v>245</v>
       </c>
       <c r="S120" s="13" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
       <c r="T120" s="13" t="s">
         <v>54</v>
@@ -17345,7 +17325,7 @@
         <v>244</v>
       </c>
       <c r="P121" s="13" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
       <c r="Q121" s="13" t="s">
         <v>243</v>
@@ -17354,7 +17334,7 @@
         <v>245</v>
       </c>
       <c r="S121" s="13" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
       <c r="T121" s="13" t="s">
         <v>54</v>
@@ -17444,7 +17424,7 @@
         <v>244</v>
       </c>
       <c r="P122" s="13" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
       <c r="Q122" s="13" t="s">
         <v>243</v>
@@ -17453,7 +17433,7 @@
         <v>245</v>
       </c>
       <c r="S122" s="13" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
       <c r="T122" s="13" t="s">
         <v>54</v>
@@ -17537,7 +17517,7 @@
         <v>244</v>
       </c>
       <c r="P123" s="13" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
       <c r="Q123" s="13" t="s">
         <v>243</v>
@@ -17546,7 +17526,7 @@
         <v>245</v>
       </c>
       <c r="S123" s="13" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
       <c r="T123" s="13" t="s">
         <v>54</v>
@@ -17636,7 +17616,7 @@
         <v>244</v>
       </c>
       <c r="P124" s="13" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
       <c r="Q124" s="13" t="s">
         <v>243</v>
@@ -17645,7 +17625,7 @@
         <v>245</v>
       </c>
       <c r="S124" s="13" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
       <c r="T124" s="13" t="s">
         <v>54</v>
@@ -17729,7 +17709,7 @@
         <v>244</v>
       </c>
       <c r="P125" s="13" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
       <c r="Q125" s="13" t="s">
         <v>243</v>
@@ -17738,7 +17718,7 @@
         <v>245</v>
       </c>
       <c r="S125" s="13" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
       <c r="T125" s="13" t="s">
         <v>54</v>
@@ -17822,7 +17802,7 @@
         <v>244</v>
       </c>
       <c r="P126" s="13" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
       <c r="Q126" s="13" t="s">
         <v>243</v>
@@ -17831,7 +17811,7 @@
         <v>245</v>
       </c>
       <c r="S126" s="13" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
       <c r="T126" s="13" t="s">
         <v>54</v>
@@ -17915,7 +17895,7 @@
         <v>244</v>
       </c>
       <c r="P127" s="13" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
       <c r="Q127" s="13" t="s">
         <v>243</v>
@@ -17924,7 +17904,7 @@
         <v>245</v>
       </c>
       <c r="S127" s="13" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
       <c r="T127" s="13" t="s">
         <v>54</v>
@@ -18008,7 +17988,7 @@
         <v>244</v>
       </c>
       <c r="P128" s="13" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
       <c r="Q128" s="13" t="s">
         <v>243</v>
@@ -18017,7 +17997,7 @@
         <v>245</v>
       </c>
       <c r="S128" s="13" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
       <c r="T128" s="13" t="s">
         <v>54</v>
@@ -18101,7 +18081,7 @@
         <v>244</v>
       </c>
       <c r="P129" s="13" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
       <c r="Q129" s="13" t="s">
         <v>243</v>
@@ -18110,7 +18090,7 @@
         <v>245</v>
       </c>
       <c r="S129" s="13" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
       <c r="T129" s="13" t="s">
         <v>54</v>
@@ -18194,7 +18174,7 @@
         <v>244</v>
       </c>
       <c r="P130" s="13" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
       <c r="Q130" s="13" t="s">
         <v>243</v>
@@ -18203,7 +18183,7 @@
         <v>245</v>
       </c>
       <c r="S130" s="13" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
       <c r="T130" s="13" t="s">
         <v>54</v>

</xml_diff>

<commit_message>
Excel Format Updated as per latest config
</commit_message>
<xml_diff>
--- a/Excels/KE.xlsx
+++ b/Excels/KE.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2394650\IdeaProjects\cs-portal-automation_selenium1\Excels\"/>
     </mc:Choice>
@@ -19,18 +19,18 @@
     <sheet name="FTRTickets-San" sheetId="2" r:id="rId5"/>
     <sheet name="NFTRTickets-Reg" sheetId="11" r:id="rId6"/>
     <sheet name="FTRTickets-Reg" sheetId="12" r:id="rId7"/>
-    <sheet name="WorkFlows" sheetId="7" r:id="rId8"/>
-    <sheet name="LoginQueue" sheetId="8" r:id="rId9"/>
-    <sheet name="PinnedTags" sheetId="5" r:id="rId10"/>
-    <sheet name="InteractionChannel" sheetId="4" r:id="rId11"/>
-    <sheet name="Ticket State" sheetId="6" r:id="rId12"/>
-    <sheet name="Ticket Transfer Rules" sheetId="15" r:id="rId13"/>
-    <sheet name="Authentication Policy" sheetId="17" r:id="rId14"/>
-    <sheet name="Action Tagging" sheetId="18" r:id="rId15"/>
+    <sheet name="UserManagement" sheetId="19" r:id="rId8"/>
+    <sheet name="PinnedTags" sheetId="5" r:id="rId9"/>
+    <sheet name="Ticket State" sheetId="6" r:id="rId10"/>
+    <sheet name="TemplateManagement" sheetId="20" r:id="rId11"/>
+    <sheet name="Ticket Transfer Rules" sheetId="15" r:id="rId12"/>
+    <sheet name="Authentication Policy" sheetId="17" r:id="rId13"/>
+    <sheet name="Action Tagging" sheetId="18" r:id="rId14"/>
+    <sheet name="State Queue Mapping" sheetId="21" r:id="rId15"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3555" uniqueCount="1045">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3590" uniqueCount="1068">
   <si>
     <t>loginAuuid</t>
   </si>
@@ -3200,14 +3200,91 @@
   <si>
     <t>Category code</t>
   </si>
+  <si>
+    <t>Customer Service Backend Supervisor</t>
+  </si>
+  <si>
+    <t>Advisor Supervisor</t>
+  </si>
+  <si>
+    <t>Customer Service Frontend Agent</t>
+  </si>
+  <si>
+    <t>Swahili</t>
+  </si>
+  <si>
+    <t>Customer Service Backend Agent</t>
+  </si>
+  <si>
+    <t>French</t>
+  </si>
+  <si>
+    <t>CS SMS Management</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>CS Profile Management</t>
+  </si>
+  <si>
+    <t>Langugae</t>
+  </si>
+  <si>
+    <t>Roles</t>
+  </si>
+  <si>
+    <t>Queue Name</t>
+  </si>
+  <si>
+    <t>State name1</t>
+  </si>
+  <si>
+    <t>State name2</t>
+  </si>
+  <si>
+    <t>State name3</t>
+  </si>
+  <si>
+    <t>State name4</t>
+  </si>
+  <si>
+    <t>State name5</t>
+  </si>
+  <si>
+    <t>State name6</t>
+  </si>
+  <si>
+    <t>State name7</t>
+  </si>
+  <si>
+    <t>State name8</t>
+  </si>
+  <si>
+    <t>State name9</t>
+  </si>
+  <si>
+    <t>State name10</t>
+  </si>
+  <si>
+    <t>141020001898</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -3272,7 +3349,7 @@
       <name val="Verdana"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3315,8 +3392,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -3378,25 +3461,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -3410,77 +3507,86 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
     <cellStyle name="Normal 3" xfId="2"/>
+    <cellStyle name="Normal 4" xfId="3"/>
   </cellStyles>
   <dxfs count="8">
     <dxf>
@@ -3596,7 +3702,7 @@
         <xdr:cNvPr id="9217" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{954E16FB-6A94-A343-90CA-E894AD77BEF0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{954E16FB-6A94-A343-90CA-E894AD77BEF0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3934,11 +4040,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="17.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="8" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="20.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="17.125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="14.5" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="13.125" collapsed="true"/>
+    <col min="7" max="8" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="20.375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
@@ -4114,125 +4220,6 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" s="1">
-        <v>735873718</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" s="1">
-        <v>735873718</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" s="1">
-        <v>735873718</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="28.375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18.625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="17.125" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="7"/>
@@ -4245,9 +4232,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="24.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="14.875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="16.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -4382,20 +4369,86 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J13" activeCellId="1" sqref="I1 J13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" style="47" width="30.875" collapsed="true"/>
+    <col min="2" max="16384" style="47" width="9.0" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="48" t="s">
+        <v>1055</v>
+      </c>
+      <c r="B1" s="48" t="s">
+        <v>1054</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="47" t="s">
+        <v>1053</v>
+      </c>
+      <c r="B2" s="47" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="47" t="s">
+        <v>1051</v>
+      </c>
+      <c r="B3" s="47" t="s">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="47" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B4" s="47" t="s">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="47" t="s">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="47" t="s">
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="47" t="s">
+        <v>1045</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="37.25" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="27.75" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="13.375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="37.25" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="20.125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="27.75" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -5882,7 +5935,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2"/>
   <sheetViews>
@@ -5892,19 +5945,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="15.875" style="8" customWidth="1"/>
-    <col min="3" max="3" width="19.75" style="8" customWidth="1"/>
-    <col min="4" max="4" width="10.875" style="44" customWidth="1"/>
-    <col min="5" max="5" width="11.5" style="44" customWidth="1"/>
-    <col min="6" max="6" width="10.125" style="44" customWidth="1"/>
-    <col min="7" max="7" width="10" style="44" customWidth="1"/>
-    <col min="8" max="8" width="11" style="44" customWidth="1"/>
-    <col min="9" max="9" width="10.25" style="44" customWidth="1"/>
-    <col min="10" max="10" width="10.125" style="44" customWidth="1"/>
-    <col min="11" max="11" width="10.5" style="44" customWidth="1"/>
-    <col min="12" max="12" width="11.625" style="44" customWidth="1"/>
-    <col min="13" max="13" width="11.875" style="44" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="12.0" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" style="8" width="15.875" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" style="8" width="19.75" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" style="44" width="10.875" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" style="44" width="11.5" collapsed="false"/>
+    <col min="6" max="6" customWidth="true" style="44" width="10.125" collapsed="false"/>
+    <col min="7" max="7" customWidth="true" style="44" width="10.0" collapsed="false"/>
+    <col min="8" max="8" customWidth="true" style="44" width="11.0" collapsed="false"/>
+    <col min="9" max="9" customWidth="true" style="44" width="10.25" collapsed="false"/>
+    <col min="10" max="10" customWidth="true" style="44" width="10.125" collapsed="false"/>
+    <col min="11" max="11" customWidth="true" style="44" width="10.5" collapsed="false"/>
+    <col min="12" max="12" customWidth="true" style="44" width="11.625" collapsed="false"/>
+    <col min="13" max="13" customWidth="true" style="44" width="11.875" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
@@ -5984,19 +6037,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.375" customWidth="1"/>
-    <col min="3" max="3" width="11" customWidth="1"/>
-    <col min="7" max="7" width="14" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="13.375" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="11.0" collapsed="false"/>
+    <col min="7" max="7" customWidth="true" width="14.0" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -6032,6 +6085,127 @@
       <c r="C2" t="s">
         <v>1040</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" style="50" width="19.25" collapsed="false"/>
+    <col min="2" max="2" style="50" width="9.0" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" style="50" width="13.875" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" style="50" width="11.5" collapsed="false"/>
+    <col min="5" max="16384" style="50" width="9.0" collapsed="false"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="49" t="s">
+        <v>1056</v>
+      </c>
+      <c r="B1" s="49" t="s">
+        <v>1057</v>
+      </c>
+      <c r="C1" s="49" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D1" s="49" t="s">
+        <v>1059</v>
+      </c>
+      <c r="E1" s="49" t="s">
+        <v>1060</v>
+      </c>
+      <c r="F1" s="49" t="s">
+        <v>1061</v>
+      </c>
+      <c r="G1" s="49" t="s">
+        <v>1062</v>
+      </c>
+      <c r="H1" s="49" t="s">
+        <v>1063</v>
+      </c>
+      <c r="I1" s="49" t="s">
+        <v>1064</v>
+      </c>
+      <c r="J1" s="49" t="s">
+        <v>1065</v>
+      </c>
+      <c r="K1" s="49" t="s">
+        <v>1066</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="51" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" s="49" t="s">
+        <v>114</v>
+      </c>
+      <c r="C2" s="52" t="s">
+        <v>119</v>
+      </c>
+      <c r="D2" s="52" t="s">
+        <v>118</v>
+      </c>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+    </row>
+    <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="49" t="s">
+        <v>114</v>
+      </c>
+      <c r="C3" s="52" t="s">
+        <v>119</v>
+      </c>
+      <c r="D3" s="52" t="s">
+        <v>118</v>
+      </c>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="49"/>
+    </row>
+    <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4" s="49" t="s">
+        <v>114</v>
+      </c>
+      <c r="C4" s="52" t="s">
+        <v>119</v>
+      </c>
+      <c r="D4" s="52" t="s">
+        <v>118</v>
+      </c>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="49"/>
+      <c r="H4" s="49"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="49"/>
+      <c r="K4" s="49"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6049,7 +6223,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="16.625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -6102,15 +6276,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="21.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="22.375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="7.375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="29.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="12.375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.5" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="21.5" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="22.375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="7.375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -6329,7 +6503,7 @@
       <c r="I9" s="1"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
@@ -6338,7 +6512,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE3"/>
+  <dimension ref="A1:AL3"/>
   <sheetViews>
     <sheetView topLeftCell="X1" zoomScale="125" workbookViewId="0">
       <selection activeCell="V4" sqref="V4"/>
@@ -6346,30 +6520,30 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="23.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18.625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="17.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="17.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="17.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="17.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="17.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="23.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="17.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="23.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="26" width="23.875" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="9.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="3" max="4" bestFit="true" customWidth="true" width="23.875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="18.625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="12.375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="12.375" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="12.375" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="12.375" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="12.375" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="23.875" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="23.875" collapsed="true"/>
+    <col min="24" max="26" customWidth="true" width="23.875" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="9.875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -6542,6 +6716,9 @@
       </c>
       <c r="AE2" t="s">
         <v>1012</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>1067</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
@@ -6591,10 +6768,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="28.625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="24.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.5" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="28.625" collapsed="true"/>
+    <col min="3" max="4" bestFit="true" customWidth="true" width="24.5" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="18.625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -6666,7 +6843,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="21" max="26" width="9" style="8" collapsed="1"/>
+    <col min="21" max="26" style="8" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
@@ -17981,89 +18158,185 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A15"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="17.125" collapsed="false"/>
+    <col min="2" max="3" bestFit="true" customWidth="true" width="22.625" collapsed="false"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="45" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="45" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C1" s="45" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" s="46" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B3" s="46" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C3" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B4" s="46" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C4" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B5" s="46" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="C5" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="46" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="C6" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="46" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="C7" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="46" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="C8" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="46" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="C9" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="46" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="C10" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="46" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="C11" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="46" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="C12" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="46" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="C13" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="46" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="C14" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="46" t="s">
+        <v>201</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C16" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C17" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C18" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C19" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C20" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C21" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C22" s="1" t="s">
         <v>201</v>
       </c>
     </row>
@@ -18074,125 +18347,72 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A22"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>201</v>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="1">
+        <v>735873718</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="1">
+        <v>735873718</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="1">
+        <v>735873718</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fluent Wait Implementation and handle DOM Creation Using Fluent wait
</commit_message>
<xml_diff>
--- a/Excels/KE.xlsx
+++ b/Excels/KE.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2394650\IdeaProjects\cs-portal-automation_selenium1\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="35835" windowHeight="20205" firstSheet="12" activeTab="15"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="35835" windowHeight="20205" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="LoginCredentials" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3584" uniqueCount="1008">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3599" uniqueCount="1023">
   <si>
     <t>loginAuuid</t>
   </si>
@@ -3089,11 +3089,57 @@
   <si>
     <t>520920001740</t>
   </si>
+  <si>
+    <t>101120002601</t>
+  </si>
+  <si>
+    <t>101120002602</t>
+  </si>
+  <si>
+    <t>101120002604</t>
+  </si>
+  <si>
+    <t>101120002605</t>
+  </si>
+  <si>
+    <t>101120002607</t>
+  </si>
+  <si>
+    <t>101120002608</t>
+  </si>
+  <si>
+    <t>101120002609</t>
+  </si>
+  <si>
+    <t>101120002611</t>
+  </si>
+  <si>
+    <t>101120002612</t>
+  </si>
+  <si>
+    <t>101120002614</t>
+  </si>
+  <si>
+    <t>101120002615</t>
+  </si>
+  <si>
+    <t>101120002617</t>
+  </si>
+  <si>
+    <t>101120002618</t>
+  </si>
+  <si>
+    <t>101120002619</t>
+  </si>
+  <si>
+    <t>101120002620</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -3515,7 +3561,7 @@
         <xdr:cNvPr id="9217" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{954E16FB-6A94-A343-90CA-E894AD77BEF0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{954E16FB-6A94-A343-90CA-E894AD77BEF0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3853,11 +3899,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="17.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="8" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="20.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="17.125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="14.5" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="13.125" collapsed="true"/>
+    <col min="7" max="8" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="20.375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
@@ -4045,9 +4091,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="24.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="14.875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="16.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -4192,8 +4238,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.875" style="44" customWidth="1" collapsed="1"/>
-    <col min="2" max="16384" width="9" style="44" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="44" width="30.875" collapsed="true"/>
+    <col min="2" max="16384" style="44" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -4258,10 +4304,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="37.25" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="27.75" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="13.375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="37.25" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="20.125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="27.75" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -5758,19 +5804,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="15.875" style="7" customWidth="1"/>
-    <col min="3" max="3" width="19.75" style="7" customWidth="1"/>
-    <col min="4" max="4" width="10.875" style="41" customWidth="1"/>
-    <col min="5" max="5" width="11.5" style="41" customWidth="1"/>
-    <col min="6" max="6" width="10.125" style="41" customWidth="1"/>
-    <col min="7" max="7" width="10" style="41" customWidth="1"/>
-    <col min="8" max="8" width="11" style="41" customWidth="1"/>
-    <col min="9" max="9" width="10.25" style="41" customWidth="1"/>
-    <col min="10" max="10" width="10.125" style="41" customWidth="1"/>
-    <col min="11" max="11" width="10.5" style="41" customWidth="1"/>
-    <col min="12" max="12" width="11.625" style="41" customWidth="1"/>
-    <col min="13" max="13" width="11.875" style="41" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="7" width="15.875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="7" width="19.75" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="41" width="10.875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="41" width="11.5" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="41" width="10.125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="41" width="10.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="41" width="11.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="41" width="10.25" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="41" width="10.125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="41" width="10.5" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="41" width="11.625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="41" width="11.875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
@@ -5860,9 +5906,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.375" customWidth="1"/>
-    <col min="3" max="3" width="11" customWidth="1"/>
-    <col min="7" max="7" width="14" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="13.375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -5915,11 +5961,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.25" style="47" customWidth="1"/>
-    <col min="2" max="2" width="9" style="47"/>
-    <col min="3" max="3" width="13.875" style="47" customWidth="1"/>
-    <col min="4" max="4" width="11.5" style="47" customWidth="1"/>
-    <col min="5" max="16384" width="9" style="47"/>
+    <col min="1" max="1" customWidth="true" style="47" width="19.25" collapsed="true"/>
+    <col min="2" max="2" style="47" width="9.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="47" width="13.875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="47" width="11.5" collapsed="true"/>
+    <col min="5" max="16384" style="47" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -6030,15 +6076,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.125" style="7" customWidth="1"/>
-    <col min="2" max="2" width="24.25" style="7" customWidth="1"/>
-    <col min="3" max="16384" width="9" style="7"/>
+    <col min="1" max="1" customWidth="true" style="7" width="23.125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="7" width="24.25" collapsed="true"/>
+    <col min="3" max="16384" style="7" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -6089,7 +6135,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="16.625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -6142,15 +6188,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="21.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="22.375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="12.375" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="29.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="12.375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.5" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="21.5" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="22.375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="12.375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -6474,36 +6520,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BG3"/>
   <sheetViews>
-    <sheetView topLeftCell="AU1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AU1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="AA1" sqref="AA1:BG1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="23.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18.625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="17.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="17.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="17.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="17.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="17.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="23.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="17.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="23.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="26" width="23.875" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="9.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="3" max="4" bestFit="true" customWidth="true" width="23.875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="18.625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="12.375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="12.375" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="12.375" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="12.375" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="12.375" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="23.875" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="23.875" collapsed="true"/>
+    <col min="24" max="26" customWidth="true" width="23.875" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="9.875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:59" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -6776,7 +6822,7 @@
         <v>89</v>
       </c>
       <c r="BG2" s="7" t="s">
-        <v>977</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="3" spans="1:59" x14ac:dyDescent="0.25">
@@ -6825,7 +6871,7 @@
         <v>89</v>
       </c>
       <c r="BG3" s="7" t="s">
-        <v>908</v>
+        <v>1022</v>
       </c>
     </row>
   </sheetData>
@@ -6843,10 +6889,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="28.625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="24.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.5" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="28.625" collapsed="true"/>
+    <col min="3" max="4" bestFit="true" customWidth="true" width="24.5" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="18.625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -6918,8 +6964,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="21" max="26" width="9" style="7" collapsed="1"/>
-    <col min="59" max="59" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="21" max="26" style="7" width="9.0" collapsed="true"/>
+    <col min="59" max="59" bestFit="true" customWidth="true" width="10.875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:60" x14ac:dyDescent="0.25">
@@ -18804,8 +18850,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="22.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="17.125" collapsed="true"/>
+    <col min="2" max="3" bestFit="true" customWidth="true" width="22.625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Usage History Detailed Widget API and UI Automation
</commit_message>
<xml_diff>
--- a/Excels/KE.xlsx
+++ b/Excels/KE.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="35835" windowHeight="20205"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="35835" windowHeight="20205" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="LoginCredentials" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3597" uniqueCount="1015">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3605" uniqueCount="1018">
   <si>
     <t>loginAuuid</t>
   </si>
@@ -3109,6 +3109,15 @@
   </si>
   <si>
     <t>161120002637</t>
+  </si>
+  <si>
+    <t>Detailed Usage History</t>
+  </si>
+  <si>
+    <t>Transaction Amount</t>
+  </si>
+  <si>
+    <t>Description</t>
   </si>
 </sst>
 </file>
@@ -3240,7 +3249,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -3304,6 +3313,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -3313,7 +3333,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -3415,6 +3435,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3868,8 +3889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3939,7 +3960,7 @@
         <v>124</v>
       </c>
       <c r="D2" s="7">
-        <v>735948275</v>
+        <v>751522556</v>
       </c>
       <c r="E2" t="s">
         <v>5</v>
@@ -4030,7 +4051,7 @@
         <v>131</v>
       </c>
       <c r="D4" s="5">
-        <v>735948275</v>
+        <v>751522556</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -6155,10 +6176,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6548,6 +6569,32 @@
       </c>
       <c r="K14" s="52" t="s">
         <v>158</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="55" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D15" s="55" t="s">
+        <v>150</v>
+      </c>
+      <c r="E15" s="55" t="s">
+        <v>1016</v>
+      </c>
+      <c r="F15" t="s">
+        <v>1003</v>
+      </c>
+      <c r="G15" t="s">
+        <v>1017</v>
+      </c>
+      <c r="H15" t="s">
+        <v>152</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
JSON Ignore properties added to POJO
</commit_message>
<xml_diff>
--- a/Excels/KE.xlsx
+++ b/Excels/KE.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3610" uniqueCount="1022">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3615" uniqueCount="1027">
   <si>
     <t>loginAuuid</t>
   </si>
@@ -3130,6 +3130,21 @@
   </si>
   <si>
     <t>Period</t>
+  </si>
+  <si>
+    <t>Accumulator</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>Next Reset Date</t>
   </si>
 </sst>
 </file>
@@ -3557,7 +3572,7 @@
         <xdr:cNvPr id="9217" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{954E16FB-6A94-A343-90CA-E894AD77BEF0}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{954E16FB-6A94-A343-90CA-E894AD77BEF0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6176,10 +6191,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6622,6 +6637,29 @@
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="52" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B17" s="52" t="s">
+        <v>1023</v>
+      </c>
+      <c r="C17" s="52" t="s">
+        <v>1024</v>
+      </c>
+      <c r="D17" s="52" t="s">
+        <v>1025</v>
+      </c>
+      <c r="E17" s="52" t="s">
+        <v>1026</v>
+      </c>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>

</xml_diff>

<commit_message>
NG Excel File Added
</commit_message>
<xml_diff>
--- a/Excels/KE.xlsx
+++ b/Excels/KE.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" firstSheet="11" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" firstSheet="13" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="LoginCredentials" sheetId="1" r:id="rId1"/>
@@ -4413,7 +4413,7 @@
         <xdr:cNvPr id="9217" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{954E16FB-6A94-A343-90CA-E894AD77BEF0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{954E16FB-6A94-A343-90CA-E894AD77BEF0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4746,7 +4746,7 @@
   <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5294,7 +5294,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E444"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
@@ -15530,8 +15530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BG130"/>
   <sheetViews>
-    <sheetView topLeftCell="A121" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A79" sqref="A79"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -25558,8 +25558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BG86"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:BG86"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BC6" sqref="BC6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Airtel Money Widget Menu Changes Transfer to Queue Changes Voucher Tab Bug Fix
</commit_message>
<xml_diff>
--- a/Excels/KE.xlsx
+++ b/Excels/KE.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" firstSheet="13" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="LoginCredentials" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7782" uniqueCount="1260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7781" uniqueCount="1261">
   <si>
     <t>loginAuuid</t>
   </si>
@@ -3884,6 +3884,9 @@
       </rPr>
       <t>(Ksh)</t>
     </r>
+  </si>
+  <si>
+    <t>Transfer Anyway</t>
   </si>
 </sst>
 </file>
@@ -14583,10 +14586,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -14596,36 +14599,37 @@
     <col min="3" max="16384" width="9" style="7" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>877</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>878</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
+        <v>1260</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>98</v>
+        <v>1015</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>88</v>
+      <c r="C3" s="1" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -14691,7 +14695,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E13" workbookViewId="0">
+    <sheetView topLeftCell="E13" workbookViewId="0">
       <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Backend Agent Login Failed Terminate
</commit_message>
<xml_diff>
--- a/Excels/KE.xlsx
+++ b/Excels/KE.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="LoginCredentials" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7784" uniqueCount="1264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7791" uniqueCount="1270">
   <si>
     <t>loginAuuid</t>
   </si>
@@ -3896,6 +3896,24 @@
   </si>
   <si>
     <t>RGVhdGhub3RlQDEyMw</t>
+  </si>
+  <si>
+    <t>Voucher Id</t>
+  </si>
+  <si>
+    <t>106222035384</t>
+  </si>
+  <si>
+    <t>Test Data-UAT(if Required)</t>
+  </si>
+  <si>
+    <t>Test Data-Prod</t>
+  </si>
+  <si>
+    <t>Service Details</t>
+  </si>
+  <si>
+    <t>HLR Code Detail</t>
   </si>
 </sst>
 </file>
@@ -4084,7 +4102,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -4159,6 +4177,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -4176,7 +4205,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -4335,6 +4364,7 @@
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4832,7 +4862,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -14101,10 +14131,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -14114,7 +14144,7 @@
     <col min="7" max="7" width="14" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>904</v>
       </c>
@@ -14136,8 +14166,14 @@
       <c r="G1" t="s">
         <v>913</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>1266</v>
+      </c>
+      <c r="I1" t="s">
+        <v>1267</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>905</v>
       </c>
@@ -14146,6 +14182,17 @@
       </c>
       <c r="C2" t="s">
         <v>909</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1264</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>1265</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>1265</v>
       </c>
     </row>
   </sheetData>
@@ -14750,8 +14797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17:F17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -15257,21 +15304,25 @@
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="38" t="s">
         <v>1241</v>
       </c>
       <c r="B18" s="38" t="s">
         <v>1242</v>
       </c>
-      <c r="C18" s="38" t="s">
+      <c r="C18" s="98" t="s">
+        <v>1268</v>
+      </c>
+      <c r="D18" s="38" t="s">
         <v>1243</v>
       </c>
-      <c r="D18" s="38" t="s">
-        <v>145</v>
-      </c>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
+      <c r="E18" s="98" t="s">
+        <v>1269</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>904</v>
+      </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>

</xml_diff>

<commit_message>
KE UAT User Update
</commit_message>
<xml_diff>
--- a/Excels/KE.xlsx
+++ b/Excels/KE.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155"/>
   </bookViews>
   <sheets>
     <sheet name="LoginCredentials" sheetId="1" r:id="rId1"/>
@@ -3411,9 +3411,6 @@
     <t>Airtel Money_Agent</t>
   </si>
   <si>
-    <t>QWFpcnRlbEAwOTE5</t>
-  </si>
-  <si>
     <t>080221003433</t>
   </si>
   <si>
@@ -3914,6 +3911,9 @@
   </si>
   <si>
     <t>HLR Code Detail</t>
+  </si>
+  <si>
+    <t>TWFyY2hAMTIzJA</t>
   </si>
 </sst>
 </file>
@@ -4530,7 +4530,7 @@
         <xdr:cNvPr id="9217" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{954E16FB-6A94-A343-90CA-E894AD77BEF0}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{954E16FB-6A94-A343-90CA-E894AD77BEF0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4862,8 +4862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4922,18 +4922,18 @@
         <v>174</v>
       </c>
       <c r="P1" s="1" t="s">
+        <v>1257</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>1258</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>1259</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>2388008</v>
+        <v>2390495</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1113</v>
+        <v>1269</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>124</v>
@@ -4978,7 +4978,7 @@
         <v>789474747</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -4986,7 +4986,7 @@
         <v>2394650</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>123</v>
@@ -5035,7 +5035,7 @@
         <v>2390932</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>131</v>
@@ -5058,15 +5058,15 @@
         <v>789474747</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>2388008</v>
+        <v>2390495</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>1113</v>
+        <v>1269</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>177</v>
@@ -6367,7 +6367,7 @@
         <v>1022</v>
       </c>
       <c r="D53" s="89" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="E53" s="90" t="s">
         <v>84</v>
@@ -14099,7 +14099,7 @@
         <v>897</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="C2" s="4">
         <v>3</v>
@@ -14114,7 +14114,7 @@
         <v>900</v>
       </c>
       <c r="G2" s="29" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
       <c r="H2" s="29" t="s">
         <v>901</v>
@@ -14167,10 +14167,10 @@
         <v>913</v>
       </c>
       <c r="H1" t="s">
+        <v>1265</v>
+      </c>
+      <c r="I1" t="s">
         <v>1266</v>
-      </c>
-      <c r="I1" t="s">
-        <v>1267</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -14186,13 +14186,13 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>1263</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>1264</v>
       </c>
-      <c r="H3" s="4" t="s">
-        <v>1265</v>
-      </c>
       <c r="I3" s="4" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
     </row>
   </sheetData>
@@ -14709,7 +14709,7 @@
         <v>878</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -14797,7 +14797,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
@@ -14852,10 +14852,10 @@
         <v>983</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>1250</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>1251</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>1252</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
@@ -14863,7 +14863,7 @@
         <v>77</v>
       </c>
       <c r="B2" s="39" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>142</v>
@@ -15306,19 +15306,19 @@
     </row>
     <row r="18" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="38" t="s">
+        <v>1240</v>
+      </c>
+      <c r="B18" s="38" t="s">
         <v>1241</v>
       </c>
-      <c r="B18" s="38" t="s">
+      <c r="C18" s="98" t="s">
+        <v>1267</v>
+      </c>
+      <c r="D18" s="38" t="s">
         <v>1242</v>
       </c>
-      <c r="C18" s="98" t="s">
+      <c r="E18" s="98" t="s">
         <v>1268</v>
-      </c>
-      <c r="D18" s="38" t="s">
-        <v>1243</v>
-      </c>
-      <c r="E18" s="98" t="s">
-        <v>1269</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>904</v>
@@ -15333,43 +15333,43 @@
     </row>
     <row r="19" spans="1:14" ht="42" x14ac:dyDescent="0.25">
       <c r="A19" s="38" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="B19" s="39" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
       <c r="C19" s="38" t="s">
         <v>143</v>
       </c>
       <c r="D19" s="38" t="s">
+        <v>1245</v>
+      </c>
+      <c r="E19" s="38" t="s">
         <v>1246</v>
       </c>
-      <c r="E19" s="38" t="s">
+      <c r="F19" s="38" t="s">
         <v>1247</v>
       </c>
-      <c r="F19" s="38" t="s">
+      <c r="G19" s="38" t="s">
         <v>1248</v>
-      </c>
-      <c r="G19" s="38" t="s">
-        <v>1249</v>
       </c>
       <c r="H19" s="38" t="s">
         <v>144</v>
       </c>
       <c r="I19" s="95" t="s">
+        <v>1253</v>
+      </c>
+      <c r="J19" s="95" t="s">
         <v>1254</v>
       </c>
-      <c r="J19" s="95" t="s">
+      <c r="K19" s="95" t="s">
         <v>1255</v>
-      </c>
-      <c r="K19" s="95" t="s">
-        <v>1256</v>
       </c>
       <c r="L19" s="38" t="s">
         <v>145</v>
       </c>
       <c r="M19" s="38" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
       <c r="N19" s="94"/>
     </row>
@@ -15674,7 +15674,7 @@
         <v>89</v>
       </c>
       <c r="BG2" s="2" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="3" spans="1:59" x14ac:dyDescent="0.25">
@@ -15711,7 +15711,7 @@
         <v>89</v>
       </c>
       <c r="BG3" s="2" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
     </row>
   </sheetData>
@@ -16076,7 +16076,7 @@
         <v>89</v>
       </c>
       <c r="BG2" s="1" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="3" spans="1:59" ht="38.25" x14ac:dyDescent="0.25">
@@ -16163,7 +16163,7 @@
         <v>89</v>
       </c>
       <c r="BG3" s="1" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="4" spans="1:59" ht="38.25" x14ac:dyDescent="0.25">
@@ -16244,7 +16244,7 @@
         <v>89</v>
       </c>
       <c r="BG4" s="1" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="5" spans="1:59" ht="38.25" x14ac:dyDescent="0.25">
@@ -16331,7 +16331,7 @@
         <v>89</v>
       </c>
       <c r="BG5" s="1" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="6" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -16406,7 +16406,7 @@
         <v>89</v>
       </c>
       <c r="BG6" s="1" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="7" spans="1:59" ht="38.25" x14ac:dyDescent="0.25">
@@ -16556,7 +16556,7 @@
         <v>89</v>
       </c>
       <c r="BG8" s="1" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="9" spans="1:59" ht="63.75" x14ac:dyDescent="0.25">
@@ -16631,7 +16631,7 @@
         <v>89</v>
       </c>
       <c r="BG9" s="1" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="10" spans="1:59" ht="89.25" x14ac:dyDescent="0.25">
@@ -16718,7 +16718,7 @@
         <v>89</v>
       </c>
       <c r="BG10" s="1" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="11" spans="1:59" ht="25.5" x14ac:dyDescent="0.25">
@@ -16781,7 +16781,7 @@
         <v>89</v>
       </c>
       <c r="BG11" s="1" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="12" spans="1:59" ht="63.75" x14ac:dyDescent="0.25">
@@ -16856,7 +16856,7 @@
         <v>89</v>
       </c>
       <c r="BG12" s="1" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="13" spans="1:59" ht="63.75" x14ac:dyDescent="0.25">
@@ -16931,7 +16931,7 @@
         <v>89</v>
       </c>
       <c r="BG13" s="1" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="14" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -17006,7 +17006,7 @@
         <v>89</v>
       </c>
       <c r="BG14" s="1" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="15" spans="1:59" ht="38.25" x14ac:dyDescent="0.25">
@@ -17087,7 +17087,7 @@
         <v>89</v>
       </c>
       <c r="BG15" s="1" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="16" spans="1:59" ht="63.75" x14ac:dyDescent="0.25">
@@ -17150,7 +17150,7 @@
         <v>89</v>
       </c>
       <c r="BG16" s="1" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="17" spans="1:59" ht="76.5" x14ac:dyDescent="0.25">
@@ -17213,7 +17213,7 @@
         <v>89</v>
       </c>
       <c r="BG17" s="1" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="18" spans="1:59" ht="76.5" x14ac:dyDescent="0.25">
@@ -17361,7 +17361,7 @@
         <v>89</v>
       </c>
       <c r="BG19" s="1" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="20" spans="1:59" x14ac:dyDescent="0.25">
@@ -17454,7 +17454,7 @@
         <v>89</v>
       </c>
       <c r="BG20" s="1" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="21" spans="1:59" x14ac:dyDescent="0.25">
@@ -17547,7 +17547,7 @@
         <v>89</v>
       </c>
       <c r="BG21" s="1" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="22" spans="1:59" x14ac:dyDescent="0.25">
@@ -17640,7 +17640,7 @@
         <v>89</v>
       </c>
       <c r="BG22" s="1" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="23" spans="1:59" x14ac:dyDescent="0.25">
@@ -17733,7 +17733,7 @@
         <v>89</v>
       </c>
       <c r="BG23" s="1" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="24" spans="1:59" x14ac:dyDescent="0.25">
@@ -17826,7 +17826,7 @@
         <v>89</v>
       </c>
       <c r="BG24" s="1" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="25" spans="1:59" x14ac:dyDescent="0.25">
@@ -17919,7 +17919,7 @@
         <v>89</v>
       </c>
       <c r="BG25" s="1" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="26" spans="1:59" x14ac:dyDescent="0.25">
@@ -18018,7 +18018,7 @@
         <v>89</v>
       </c>
       <c r="BG26" s="1" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="27" spans="1:59" ht="76.5" x14ac:dyDescent="0.25">
@@ -18166,7 +18166,7 @@
         <v>89</v>
       </c>
       <c r="BG28" s="1" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="29" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -18229,7 +18229,7 @@
         <v>89</v>
       </c>
       <c r="BG29" s="1" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="30" spans="1:59" ht="63.75" x14ac:dyDescent="0.25">
@@ -18292,7 +18292,7 @@
         <v>89</v>
       </c>
       <c r="BG30" s="1" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="31" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -18355,7 +18355,7 @@
         <v>89</v>
       </c>
       <c r="BG31" s="1" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="32" spans="1:59" ht="76.5" x14ac:dyDescent="0.25">
@@ -18418,7 +18418,7 @@
         <v>89</v>
       </c>
       <c r="BG32" s="1" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="33" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -18481,7 +18481,7 @@
         <v>89</v>
       </c>
       <c r="BG33" s="1" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="34" spans="1:59" ht="63.75" x14ac:dyDescent="0.25">
@@ -18568,7 +18568,7 @@
         <v>89</v>
       </c>
       <c r="BG34" s="1" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="35" spans="1:59" ht="76.5" x14ac:dyDescent="0.25">
@@ -18661,7 +18661,7 @@
         <v>89</v>
       </c>
       <c r="BG35" s="1" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="36" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -18742,7 +18742,7 @@
         <v>89</v>
       </c>
       <c r="BG36" s="1" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="37" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -18817,7 +18817,7 @@
         <v>89</v>
       </c>
       <c r="BG37" s="1" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="38" spans="1:59" ht="25.5" x14ac:dyDescent="0.25">
@@ -18892,7 +18892,7 @@
         <v>89</v>
       </c>
       <c r="BG38" s="1" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="39" spans="1:59" ht="25.5" x14ac:dyDescent="0.25">
@@ -18967,7 +18967,7 @@
         <v>89</v>
       </c>
       <c r="BG39" s="1" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="40" spans="1:59" ht="38.25" x14ac:dyDescent="0.25">
@@ -19054,7 +19054,7 @@
         <v>89</v>
       </c>
       <c r="BG40" s="1" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="41" spans="1:59" ht="63.75" x14ac:dyDescent="0.25">
@@ -19141,7 +19141,7 @@
         <v>89</v>
       </c>
       <c r="BG41" s="1" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="42" spans="1:59" ht="38.25" x14ac:dyDescent="0.25">
@@ -19204,7 +19204,7 @@
         <v>89</v>
       </c>
       <c r="BG42" s="1" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="43" spans="1:59" ht="76.5" x14ac:dyDescent="0.25">
@@ -19273,7 +19273,7 @@
         <v>89</v>
       </c>
       <c r="BG43" s="1" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="44" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -19336,7 +19336,7 @@
         <v>89</v>
       </c>
       <c r="BG44" s="1" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="45" spans="1:59" ht="76.5" x14ac:dyDescent="0.25">
@@ -19399,7 +19399,7 @@
         <v>89</v>
       </c>
       <c r="BG45" s="1" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="46" spans="1:59" ht="102" x14ac:dyDescent="0.25">
@@ -19460,7 +19460,7 @@
         <v>89</v>
       </c>
       <c r="BG46" s="1" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="47" spans="1:59" ht="25.5" x14ac:dyDescent="0.25">
@@ -19535,7 +19535,7 @@
         <v>89</v>
       </c>
       <c r="BG47" s="1" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="48" spans="1:59" ht="38.25" x14ac:dyDescent="0.25">
@@ -19598,7 +19598,7 @@
         <v>89</v>
       </c>
       <c r="BG48" s="1" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="49" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -19673,7 +19673,7 @@
         <v>89</v>
       </c>
       <c r="BG49" s="1" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="50" spans="1:59" ht="63.75" x14ac:dyDescent="0.25">
@@ -19748,7 +19748,7 @@
         <v>89</v>
       </c>
       <c r="BG50" s="1" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="51" spans="1:59" ht="76.5" x14ac:dyDescent="0.25">
@@ -19823,7 +19823,7 @@
         <v>89</v>
       </c>
       <c r="BG51" s="1" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="52" spans="1:59" ht="63.75" x14ac:dyDescent="0.25">
@@ -19898,7 +19898,7 @@
         <v>89</v>
       </c>
       <c r="BG52" s="1" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="53" spans="1:59" ht="63.75" x14ac:dyDescent="0.25">
@@ -19961,7 +19961,7 @@
         <v>89</v>
       </c>
       <c r="BG53" s="1" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="54" spans="1:59" ht="63.75" x14ac:dyDescent="0.25">
@@ -20030,7 +20030,7 @@
         <v>89</v>
       </c>
       <c r="BG54" s="1" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="55" spans="1:59" ht="76.5" x14ac:dyDescent="0.25">
@@ -20117,7 +20117,7 @@
         <v>89</v>
       </c>
       <c r="BG55" s="1" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="56" spans="1:59" ht="89.25" x14ac:dyDescent="0.25">
@@ -20180,7 +20180,7 @@
         <v>89</v>
       </c>
       <c r="BG56" s="1" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="57" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -20243,7 +20243,7 @@
         <v>89</v>
       </c>
       <c r="BG57" s="1" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="58" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -20318,7 +20318,7 @@
         <v>89</v>
       </c>
       <c r="BG58" s="1" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="59" spans="1:59" ht="63.75" x14ac:dyDescent="0.25">
@@ -20399,7 +20399,7 @@
         <v>89</v>
       </c>
       <c r="BG59" s="1" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="60" spans="1:59" ht="25.5" x14ac:dyDescent="0.25">
@@ -20480,7 +20480,7 @@
         <v>89</v>
       </c>
       <c r="BG60" s="1" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="61" spans="1:59" ht="38.25" x14ac:dyDescent="0.25">
@@ -20543,7 +20543,7 @@
         <v>89</v>
       </c>
       <c r="BG61" s="1" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="62" spans="1:59" ht="38.25" x14ac:dyDescent="0.25">
@@ -20606,7 +20606,7 @@
         <v>89</v>
       </c>
       <c r="BG62" s="1" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="63" spans="1:59" ht="38.25" x14ac:dyDescent="0.25">
@@ -20669,7 +20669,7 @@
         <v>89</v>
       </c>
       <c r="BG63" s="1" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="64" spans="1:59" ht="38.25" x14ac:dyDescent="0.25">
@@ -20732,7 +20732,7 @@
         <v>89</v>
       </c>
       <c r="BG64" s="1" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="65" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -20807,7 +20807,7 @@
         <v>89</v>
       </c>
       <c r="BG65" s="1" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="66" spans="1:59" ht="38.25" x14ac:dyDescent="0.25">
@@ -20876,7 +20876,7 @@
         <v>89</v>
       </c>
       <c r="BG66" s="1" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="67" spans="1:59" ht="38.25" x14ac:dyDescent="0.25">
@@ -20951,7 +20951,7 @@
         <v>89</v>
       </c>
       <c r="BG67" s="1" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="68" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -21014,7 +21014,7 @@
         <v>89</v>
       </c>
       <c r="BG68" s="1" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="69" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -21089,7 +21089,7 @@
         <v>89</v>
       </c>
       <c r="BG69" s="1" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="70" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -21164,7 +21164,7 @@
         <v>89</v>
       </c>
       <c r="BG70" s="1" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="71" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -21227,7 +21227,7 @@
         <v>89</v>
       </c>
       <c r="BG71" s="1" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="72" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -21296,7 +21296,7 @@
         <v>89</v>
       </c>
       <c r="BG72" s="1" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
     </row>
     <row r="73" spans="1:59" ht="63.75" x14ac:dyDescent="0.25">
@@ -21365,7 +21365,7 @@
         <v>89</v>
       </c>
       <c r="BG73" s="1" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
     </row>
     <row r="74" spans="1:59" ht="63.75" x14ac:dyDescent="0.25">
@@ -21440,7 +21440,7 @@
         <v>89</v>
       </c>
       <c r="BG74" s="1" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="75" spans="1:59" ht="63.75" x14ac:dyDescent="0.25">
@@ -21515,7 +21515,7 @@
         <v>89</v>
       </c>
       <c r="BG75" s="1" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
     </row>
     <row r="76" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -21578,7 +21578,7 @@
         <v>89</v>
       </c>
       <c r="BG76" s="1" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="77" spans="1:59" ht="25.5" x14ac:dyDescent="0.25">
@@ -21641,7 +21641,7 @@
         <v>89</v>
       </c>
       <c r="BG77" s="1" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
     </row>
     <row r="78" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -21704,7 +21704,7 @@
         <v>89</v>
       </c>
       <c r="BG78" s="1" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="79" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -21779,7 +21779,7 @@
         <v>89</v>
       </c>
       <c r="BG79" s="1" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="80" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -21842,7 +21842,7 @@
         <v>89</v>
       </c>
       <c r="BG80" s="1" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
     </row>
     <row r="81" spans="1:59" ht="38.25" x14ac:dyDescent="0.25">
@@ -21911,7 +21911,7 @@
         <v>89</v>
       </c>
       <c r="BG81" s="1" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
     </row>
     <row r="82" spans="1:59" x14ac:dyDescent="0.25">
@@ -22010,7 +22010,7 @@
         <v>89</v>
       </c>
       <c r="BG82" s="1" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
     </row>
     <row r="83" spans="1:59" x14ac:dyDescent="0.25">
@@ -22109,7 +22109,7 @@
         <v>89</v>
       </c>
       <c r="BG83" s="1" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
     </row>
     <row r="84" spans="1:59" ht="38.25" x14ac:dyDescent="0.25">
@@ -22172,7 +22172,7 @@
         <v>89</v>
       </c>
       <c r="BG84" s="1" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="85" spans="1:59" x14ac:dyDescent="0.25">
@@ -22265,7 +22265,7 @@
         <v>89</v>
       </c>
       <c r="BG85" s="1" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
     </row>
     <row r="86" spans="1:59" x14ac:dyDescent="0.25">
@@ -22358,7 +22358,7 @@
         <v>89</v>
       </c>
       <c r="BG86" s="1" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="87" spans="1:59" x14ac:dyDescent="0.25">
@@ -22457,7 +22457,7 @@
         <v>89</v>
       </c>
       <c r="BG87" s="1" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="88" spans="1:59" x14ac:dyDescent="0.25">
@@ -22550,7 +22550,7 @@
         <v>89</v>
       </c>
       <c r="BG88" s="1" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="89" spans="1:59" x14ac:dyDescent="0.25">
@@ -22649,7 +22649,7 @@
         <v>89</v>
       </c>
       <c r="BG89" s="1" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="90" spans="1:59" ht="38.25" x14ac:dyDescent="0.25">
@@ -22742,7 +22742,7 @@
         <v>89</v>
       </c>
       <c r="BG90" s="1" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="91" spans="1:59" ht="38.25" x14ac:dyDescent="0.25">
@@ -22817,7 +22817,7 @@
         <v>89</v>
       </c>
       <c r="BG91" s="1" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
     </row>
     <row r="92" spans="1:59" x14ac:dyDescent="0.25">
@@ -22892,7 +22892,7 @@
         <v>89</v>
       </c>
       <c r="BG92" s="1" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
     </row>
     <row r="93" spans="1:59" x14ac:dyDescent="0.25">
@@ -22967,7 +22967,7 @@
         <v>89</v>
       </c>
       <c r="BG93" s="1" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
     </row>
     <row r="94" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -23030,7 +23030,7 @@
         <v>89</v>
       </c>
       <c r="BG94" s="1" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="95" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -23093,7 +23093,7 @@
         <v>89</v>
       </c>
       <c r="BG95" s="1" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
     </row>
     <row r="96" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -23156,7 +23156,7 @@
         <v>89</v>
       </c>
       <c r="BG96" s="1" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
     </row>
     <row r="97" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -23219,7 +23219,7 @@
         <v>89</v>
       </c>
       <c r="BG97" s="1" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
     </row>
     <row r="98" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -23282,7 +23282,7 @@
         <v>89</v>
       </c>
       <c r="BG98" s="1" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="99" spans="1:59" ht="102" x14ac:dyDescent="0.25">
@@ -23345,7 +23345,7 @@
         <v>89</v>
       </c>
       <c r="BG99" s="1" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="100" spans="1:59" ht="38.25" x14ac:dyDescent="0.25">
@@ -23420,7 +23420,7 @@
         <v>89</v>
       </c>
       <c r="BG100" s="1" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="101" spans="1:59" ht="38.25" x14ac:dyDescent="0.25">
@@ -23495,7 +23495,7 @@
         <v>89</v>
       </c>
       <c r="BG101" s="1" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="102" spans="1:59" ht="63.75" x14ac:dyDescent="0.25">
@@ -23570,7 +23570,7 @@
         <v>89</v>
       </c>
       <c r="BG102" s="1" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="103" spans="1:59" ht="38.25" x14ac:dyDescent="0.25">
@@ -23657,7 +23657,7 @@
         <v>89</v>
       </c>
       <c r="BG103" s="1" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="104" spans="1:59" x14ac:dyDescent="0.25">
@@ -23738,7 +23738,7 @@
         <v>89</v>
       </c>
       <c r="BG104" s="40" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="105" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -23813,7 +23813,7 @@
         <v>89</v>
       </c>
       <c r="BG105" s="1" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="106" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -23888,7 +23888,7 @@
         <v>89</v>
       </c>
       <c r="BG106" s="1" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="107" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -23963,7 +23963,7 @@
         <v>89</v>
       </c>
       <c r="BG107" s="1" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
     </row>
     <row r="108" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -24038,7 +24038,7 @@
         <v>89</v>
       </c>
       <c r="BG108" s="1" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
     </row>
     <row r="109" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -24113,7 +24113,7 @@
         <v>89</v>
       </c>
       <c r="BG109" s="1" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
     </row>
     <row r="110" spans="1:59" ht="63.75" x14ac:dyDescent="0.25">
@@ -24188,7 +24188,7 @@
         <v>89</v>
       </c>
       <c r="BG110" s="1" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
     </row>
     <row r="111" spans="1:59" ht="63.75" x14ac:dyDescent="0.25">
@@ -24269,7 +24269,7 @@
         <v>89</v>
       </c>
       <c r="BG111" s="1" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
     </row>
     <row r="112" spans="1:59" ht="38.25" x14ac:dyDescent="0.25">
@@ -24362,7 +24362,7 @@
         <v>89</v>
       </c>
       <c r="BG112" s="1" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="113" spans="1:59" ht="38.25" x14ac:dyDescent="0.25">
@@ -24449,7 +24449,7 @@
         <v>89</v>
       </c>
       <c r="BG113" s="1" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="114" spans="1:59" ht="38.25" x14ac:dyDescent="0.25">
@@ -24518,7 +24518,7 @@
         <v>89</v>
       </c>
       <c r="BG114" s="1" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="115" spans="1:59" ht="38.25" x14ac:dyDescent="0.25">
@@ -24611,7 +24611,7 @@
         <v>89</v>
       </c>
       <c r="BG115" s="1" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="116" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -24704,7 +24704,7 @@
         <v>89</v>
       </c>
       <c r="BG116" s="1" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="117" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -24797,7 +24797,7 @@
         <v>89</v>
       </c>
       <c r="BG117" s="1" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="118" spans="1:59" ht="89.25" x14ac:dyDescent="0.25">
@@ -24860,7 +24860,7 @@
         <v>89</v>
       </c>
       <c r="BG118" s="1" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="119" spans="1:59" ht="76.5" x14ac:dyDescent="0.25">
@@ -24941,7 +24941,7 @@
         <v>89</v>
       </c>
       <c r="BG119" s="1" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="120" spans="1:59" ht="89.25" x14ac:dyDescent="0.25">
@@ -25028,7 +25028,7 @@
         <v>89</v>
       </c>
       <c r="BG120" s="1" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="121" spans="1:59" ht="63.75" x14ac:dyDescent="0.25">
@@ -25115,7 +25115,7 @@
         <v>89</v>
       </c>
       <c r="BG121" s="1" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="122" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -25178,7 +25178,7 @@
         <v>89</v>
       </c>
       <c r="BG122" s="1" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
     </row>
     <row r="123" spans="1:59" ht="38.25" x14ac:dyDescent="0.25">
@@ -25241,7 +25241,7 @@
         <v>89</v>
       </c>
       <c r="BG123" s="1" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
     </row>
     <row r="124" spans="1:59" ht="127.5" x14ac:dyDescent="0.25">
@@ -25304,7 +25304,7 @@
         <v>89</v>
       </c>
       <c r="BG124" s="1" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="125" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -25391,7 +25391,7 @@
         <v>89</v>
       </c>
       <c r="BG125" s="1" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="126" spans="1:59" ht="38.25" x14ac:dyDescent="0.25">
@@ -25478,7 +25478,7 @@
         <v>89</v>
       </c>
       <c r="BG126" s="1" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="127" spans="1:59" ht="63.75" x14ac:dyDescent="0.25">
@@ -25723,7 +25723,7 @@
         <v>89</v>
       </c>
       <c r="BG129" s="1" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
     </row>
     <row r="130" spans="1:59" ht="51" x14ac:dyDescent="0.25">
@@ -25798,7 +25798,7 @@
         <v>89</v>
       </c>
       <c r="BG130" s="1" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Action Trail Story Automation
</commit_message>
<xml_diff>
--- a/Excels/KE.xlsx
+++ b/Excels/KE.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" firstSheet="13" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="LoginCredentials" sheetId="1" r:id="rId1"/>
@@ -4530,7 +4530,7 @@
         <xdr:cNvPr id="9217" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{954E16FB-6A94-A343-90CA-E894AD77BEF0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{954E16FB-6A94-A343-90CA-E894AD77BEF0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4862,7 +4862,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -14030,8 +14030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -14102,7 +14102,7 @@
         <v>1260</v>
       </c>
       <c r="C2" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D2" s="29" t="s">
         <v>898</v>

</xml_diff>